<commit_message>
tagit fram källor till antons körning
</commit_message>
<xml_diff>
--- a/masterProject/test.xlsx
+++ b/masterProject/test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="66">
   <si>
     <t>index</t>
   </si>
@@ -193,6 +193,27 @@
   </si>
   <si>
     <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
   </si>
 </sst>
 </file>
@@ -8010,7 +8031,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:AA35"/>
+  <dimension ref="A2:AA42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8106,28 +8127,28 @@
         <v>26</v>
       </c>
       <c r="C3" t="n">
-        <v>3.098781806768344</v>
+        <v>3.091953233214828</v>
       </c>
       <c r="D3" t="n">
-        <v>15.56905217381975</v>
+        <v>15.53474371825335</v>
       </c>
       <c r="E3" t="n">
-        <v>4.391145491801997</v>
+        <v>4.381469027154793</v>
       </c>
       <c r="F3" t="n">
-        <v>12.30371519696158</v>
+        <v>12.46926825473622</v>
       </c>
       <c r="G3" t="n">
-        <v>32.26391286258333</v>
+        <v>32.38548100014435</v>
       </c>
       <c r="H3" t="n">
-        <v>26.6699201341758</v>
+        <v>26.83230490006357</v>
       </c>
       <c r="I3" t="n">
-        <v>8.785734478150854</v>
+        <v>8.604923556260086</v>
       </c>
       <c r="J3" t="n">
-        <v>0.5072449932865355</v>
+        <v>0.5118520423414292</v>
       </c>
       <c r="K3" t="n">
         <v>1.182483619818803</v>
@@ -8136,49 +8157,49 @@
         <v>1.180312308138719</v>
       </c>
       <c r="M3" t="n">
-        <v>1.557447114779901</v>
+        <v>1.557447115290403</v>
       </c>
       <c r="N3" t="n">
-        <v>0.7793008699747366</v>
+        <v>0.6279803126980887</v>
       </c>
       <c r="O3" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="P3" t="n">
-        <v>3.191741749743329</v>
+        <v>3.0517474561793</v>
       </c>
       <c r="Q3" t="n">
-        <v>3.098781806768344</v>
+        <v>3.091953233214828</v>
       </c>
       <c r="R3" t="n">
-        <v>63.52890051600951</v>
+        <v>63.38890622244548</v>
       </c>
       <c r="S3" t="n">
-        <v>0.5624853349808941</v>
+        <v>0.4532648815865458</v>
       </c>
       <c r="T3" t="n">
-        <v>0.8124853349808941</v>
+        <v>0.7032648815865458</v>
       </c>
       <c r="U3" t="n">
         <v>0.08023942777181295</v>
       </c>
       <c r="V3" t="n">
-        <v>-0.1539964378800733</v>
+        <v>-0.1911040132728621</v>
       </c>
       <c r="W3" t="n">
-        <v>33.04660318715646</v>
+        <v>33.01685076744086</v>
       </c>
       <c r="X3" t="n">
-        <v>19.96019766562175</v>
+        <v>19.91621274540815</v>
       </c>
       <c r="Y3" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="Z3" t="n">
-        <v>2.73775942291862</v>
+        <v>2.737759423429122</v>
       </c>
       <c r="AA3" t="n">
-        <v>12.75430806918788</v>
+        <v>12.77986683288798</v>
       </c>
     </row>
     <row r="4" spans="1:27">
@@ -8189,28 +8210,28 @@
         <v>27</v>
       </c>
       <c r="C4" t="n">
-        <v>3.098781806768344</v>
+        <v>3.091953233214828</v>
       </c>
       <c r="D4" t="n">
-        <v>15.56905217381975</v>
+        <v>15.53474371825335</v>
       </c>
       <c r="E4" t="n">
-        <v>4.391145491801997</v>
+        <v>4.381469027154793</v>
       </c>
       <c r="F4" t="n">
-        <v>12.30371519696158</v>
+        <v>12.46926825473622</v>
       </c>
       <c r="G4" t="n">
-        <v>32.26391286258333</v>
+        <v>32.38548100014435</v>
       </c>
       <c r="H4" t="n">
-        <v>26.6699201341758</v>
+        <v>26.83230490006357</v>
       </c>
       <c r="I4" t="n">
-        <v>8.785734478150854</v>
+        <v>8.604923556260086</v>
       </c>
       <c r="J4" t="n">
-        <v>0.5072449932865355</v>
+        <v>0.5118520423414292</v>
       </c>
       <c r="K4" t="n">
         <v>1.182483619818803</v>
@@ -8219,49 +8240,49 @@
         <v>1.180312308138719</v>
       </c>
       <c r="M4" t="n">
-        <v>1.557447114779901</v>
+        <v>1.557447115290403</v>
       </c>
       <c r="N4" t="n">
-        <v>0.7793008699747366</v>
+        <v>0.6279803126980887</v>
       </c>
       <c r="O4" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="P4" t="n">
-        <v>3.191741749743329</v>
+        <v>3.0517474561793</v>
       </c>
       <c r="Q4" t="n">
-        <v>3.098781806768344</v>
+        <v>3.091953233214828</v>
       </c>
       <c r="R4" t="n">
-        <v>63.52890051600951</v>
+        <v>63.38890622244548</v>
       </c>
       <c r="S4" t="n">
-        <v>0.5624853349808941</v>
+        <v>0.4532648815865458</v>
       </c>
       <c r="T4" t="n">
-        <v>0.8124853349808941</v>
+        <v>0.7032648815865458</v>
       </c>
       <c r="U4" t="n">
         <v>0.08023942777181295</v>
       </c>
       <c r="V4" t="n">
-        <v>-0.1539964378800733</v>
+        <v>-0.1911040132728621</v>
       </c>
       <c r="W4" t="n">
-        <v>33.04660318715646</v>
+        <v>33.01685076744086</v>
       </c>
       <c r="X4" t="n">
-        <v>19.96019766562175</v>
+        <v>19.91621274540815</v>
       </c>
       <c r="Y4" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="Z4" t="n">
-        <v>2.73775942291862</v>
+        <v>2.737759423429122</v>
       </c>
       <c r="AA4" t="n">
-        <v>12.75430806918788</v>
+        <v>12.77986683288798</v>
       </c>
     </row>
     <row r="5" spans="1:27">
@@ -8272,28 +8293,28 @@
         <v>28</v>
       </c>
       <c r="C5" t="n">
-        <v>3.098781806768344</v>
+        <v>3.091953233214828</v>
       </c>
       <c r="D5" t="n">
-        <v>15.56905217381975</v>
+        <v>15.53474371825335</v>
       </c>
       <c r="E5" t="n">
-        <v>4.391145491801997</v>
+        <v>4.381469027154793</v>
       </c>
       <c r="F5" t="n">
-        <v>12.30371519696158</v>
+        <v>12.46926825473622</v>
       </c>
       <c r="G5" t="n">
-        <v>32.26391286258333</v>
+        <v>32.38548100014435</v>
       </c>
       <c r="H5" t="n">
-        <v>26.6699201341758</v>
+        <v>26.83230490006357</v>
       </c>
       <c r="I5" t="n">
-        <v>8.785734478150854</v>
+        <v>8.604923556260086</v>
       </c>
       <c r="J5" t="n">
-        <v>0.5072449932865355</v>
+        <v>0.5118520423414292</v>
       </c>
       <c r="K5" t="n">
         <v>1.182483619818803</v>
@@ -8302,49 +8323,49 @@
         <v>1.180312308138719</v>
       </c>
       <c r="M5" t="n">
-        <v>1.557447114779901</v>
+        <v>1.557447115290403</v>
       </c>
       <c r="N5" t="n">
-        <v>0.7793008699747366</v>
+        <v>0.6279803126980887</v>
       </c>
       <c r="O5" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="P5" t="n">
-        <v>3.191741749743329</v>
+        <v>3.0517474561793</v>
       </c>
       <c r="Q5" t="n">
-        <v>3.098781806768344</v>
+        <v>3.091953233214828</v>
       </c>
       <c r="R5" t="n">
-        <v>63.52890051600951</v>
+        <v>63.38890622244548</v>
       </c>
       <c r="S5" t="n">
-        <v>0.5624853349808941</v>
+        <v>0.4532648815865458</v>
       </c>
       <c r="T5" t="n">
-        <v>0.8124853349808941</v>
+        <v>0.7032648815865458</v>
       </c>
       <c r="U5" t="n">
         <v>0.08023942777181295</v>
       </c>
       <c r="V5" t="n">
-        <v>-0.1539964378800733</v>
+        <v>-0.1911040132728621</v>
       </c>
       <c r="W5" t="n">
-        <v>33.04660318715646</v>
+        <v>33.01685076744086</v>
       </c>
       <c r="X5" t="n">
-        <v>19.96019766562175</v>
+        <v>19.91621274540815</v>
       </c>
       <c r="Y5" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="Z5" t="n">
-        <v>2.73775942291862</v>
+        <v>2.737759423429122</v>
       </c>
       <c r="AA5" t="n">
-        <v>12.75430806918788</v>
+        <v>12.77986683288798</v>
       </c>
     </row>
     <row r="6" spans="1:27">
@@ -8355,28 +8376,28 @@
         <v>29</v>
       </c>
       <c r="C6" t="n">
-        <v>3.098781806768344</v>
+        <v>3.091953233214828</v>
       </c>
       <c r="D6" t="n">
-        <v>15.56905217381975</v>
+        <v>15.53474371825335</v>
       </c>
       <c r="E6" t="n">
-        <v>4.391145491801997</v>
+        <v>4.381469027154793</v>
       </c>
       <c r="F6" t="n">
-        <v>12.30371519696158</v>
+        <v>12.46926825473622</v>
       </c>
       <c r="G6" t="n">
-        <v>32.26391286258333</v>
+        <v>32.38548100014435</v>
       </c>
       <c r="H6" t="n">
-        <v>26.6699201341758</v>
+        <v>26.83230490006357</v>
       </c>
       <c r="I6" t="n">
-        <v>8.785734478150854</v>
+        <v>8.604923556260086</v>
       </c>
       <c r="J6" t="n">
-        <v>0.5072449932865355</v>
+        <v>0.5118520423414292</v>
       </c>
       <c r="K6" t="n">
         <v>1.182483619818803</v>
@@ -8385,49 +8406,49 @@
         <v>1.180312308138719</v>
       </c>
       <c r="M6" t="n">
-        <v>1.557447114779901</v>
+        <v>1.557447115290403</v>
       </c>
       <c r="N6" t="n">
-        <v>0.7793008699747366</v>
+        <v>0.6279803126980887</v>
       </c>
       <c r="O6" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="P6" t="n">
-        <v>3.191741749743329</v>
+        <v>3.0517474561793</v>
       </c>
       <c r="Q6" t="n">
-        <v>3.098781806768344</v>
+        <v>3.091953233214828</v>
       </c>
       <c r="R6" t="n">
-        <v>63.52890051600951</v>
+        <v>63.38890622244548</v>
       </c>
       <c r="S6" t="n">
-        <v>0.5624853349808941</v>
+        <v>0.4532648815865458</v>
       </c>
       <c r="T6" t="n">
-        <v>0.8124853349808941</v>
+        <v>0.7032648815865458</v>
       </c>
       <c r="U6" t="n">
         <v>0.08023942777181295</v>
       </c>
       <c r="V6" t="n">
-        <v>-0.1539964378800733</v>
+        <v>-0.1911040132728621</v>
       </c>
       <c r="W6" t="n">
-        <v>33.04660318715646</v>
+        <v>33.01685076744086</v>
       </c>
       <c r="X6" t="n">
-        <v>19.96019766562175</v>
+        <v>19.91621274540815</v>
       </c>
       <c r="Y6" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="Z6" t="n">
-        <v>2.73775942291862</v>
+        <v>2.737759423429122</v>
       </c>
       <c r="AA6" t="n">
-        <v>12.75430806918788</v>
+        <v>12.77986683288798</v>
       </c>
     </row>
     <row r="7" spans="1:27">
@@ -8438,28 +8459,28 @@
         <v>30</v>
       </c>
       <c r="C7" t="n">
-        <v>3.098781806768344</v>
+        <v>3.091953233214828</v>
       </c>
       <c r="D7" t="n">
-        <v>15.56905217381975</v>
+        <v>15.53474371825335</v>
       </c>
       <c r="E7" t="n">
-        <v>4.391145491801997</v>
+        <v>4.381469027154793</v>
       </c>
       <c r="F7" t="n">
-        <v>12.30371519696158</v>
+        <v>12.46926825473622</v>
       </c>
       <c r="G7" t="n">
-        <v>32.26391286258333</v>
+        <v>32.38548100014435</v>
       </c>
       <c r="H7" t="n">
-        <v>26.6699201341758</v>
+        <v>26.83230490006357</v>
       </c>
       <c r="I7" t="n">
-        <v>8.785734478150854</v>
+        <v>8.604923556260086</v>
       </c>
       <c r="J7" t="n">
-        <v>0.5072449932865355</v>
+        <v>0.5118520423414292</v>
       </c>
       <c r="K7" t="n">
         <v>1.182483619818803</v>
@@ -8468,49 +8489,49 @@
         <v>1.180312308138719</v>
       </c>
       <c r="M7" t="n">
-        <v>1.557447114779901</v>
+        <v>1.557447115290403</v>
       </c>
       <c r="N7" t="n">
-        <v>0.7793008699747366</v>
+        <v>0.6279803126980887</v>
       </c>
       <c r="O7" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="P7" t="n">
-        <v>3.191741749743329</v>
+        <v>3.0517474561793</v>
       </c>
       <c r="Q7" t="n">
-        <v>3.098781806768344</v>
+        <v>3.091953233214828</v>
       </c>
       <c r="R7" t="n">
-        <v>63.52890051600951</v>
+        <v>63.38890622244548</v>
       </c>
       <c r="S7" t="n">
-        <v>0.5624853349808941</v>
+        <v>0.4532648815865458</v>
       </c>
       <c r="T7" t="n">
-        <v>0.8124853349808941</v>
+        <v>0.7032648815865458</v>
       </c>
       <c r="U7" t="n">
         <v>0.08023942777181295</v>
       </c>
       <c r="V7" t="n">
-        <v>-0.1539964378800733</v>
+        <v>-0.1911040132728621</v>
       </c>
       <c r="W7" t="n">
-        <v>33.04660318715646</v>
+        <v>33.01685076744086</v>
       </c>
       <c r="X7" t="n">
-        <v>19.96019766562175</v>
+        <v>19.91621274540815</v>
       </c>
       <c r="Y7" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="Z7" t="n">
-        <v>2.73775942291862</v>
+        <v>2.737759423429122</v>
       </c>
       <c r="AA7" t="n">
-        <v>12.75430806918788</v>
+        <v>12.77986683288798</v>
       </c>
     </row>
     <row r="8" spans="1:27">
@@ -8521,28 +8542,28 @@
         <v>31</v>
       </c>
       <c r="C8" t="n">
-        <v>3.098781806768344</v>
+        <v>3.091953233214828</v>
       </c>
       <c r="D8" t="n">
-        <v>15.56905217381975</v>
+        <v>15.53474371825335</v>
       </c>
       <c r="E8" t="n">
-        <v>4.391145491801997</v>
+        <v>4.381469027154793</v>
       </c>
       <c r="F8" t="n">
-        <v>12.30371519696158</v>
+        <v>12.46926825473622</v>
       </c>
       <c r="G8" t="n">
-        <v>32.26391286258333</v>
+        <v>32.38548100014435</v>
       </c>
       <c r="H8" t="n">
-        <v>26.6699201341758</v>
+        <v>26.83230490006357</v>
       </c>
       <c r="I8" t="n">
-        <v>8.785734478150854</v>
+        <v>8.604923556260086</v>
       </c>
       <c r="J8" t="n">
-        <v>0.5072449932865355</v>
+        <v>0.5118520423414292</v>
       </c>
       <c r="K8" t="n">
         <v>1.182483619818803</v>
@@ -8551,49 +8572,49 @@
         <v>1.180312308138719</v>
       </c>
       <c r="M8" t="n">
-        <v>1.557447114779901</v>
+        <v>1.557447115290403</v>
       </c>
       <c r="N8" t="n">
-        <v>0.7793008699747366</v>
+        <v>0.6279803126980887</v>
       </c>
       <c r="O8" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="P8" t="n">
-        <v>3.191741749743329</v>
+        <v>3.0517474561793</v>
       </c>
       <c r="Q8" t="n">
-        <v>3.098781806768344</v>
+        <v>3.091953233214828</v>
       </c>
       <c r="R8" t="n">
-        <v>63.52890051600951</v>
+        <v>63.38890622244548</v>
       </c>
       <c r="S8" t="n">
-        <v>0.5624853349808941</v>
+        <v>0.4532648815865458</v>
       </c>
       <c r="T8" t="n">
-        <v>0.8124853349808941</v>
+        <v>0.7032648815865458</v>
       </c>
       <c r="U8" t="n">
         <v>0.08023942777181295</v>
       </c>
       <c r="V8" t="n">
-        <v>-0.1539964378800733</v>
+        <v>-0.1911040132728621</v>
       </c>
       <c r="W8" t="n">
-        <v>33.04660318715646</v>
+        <v>33.01685076744086</v>
       </c>
       <c r="X8" t="n">
-        <v>19.96019766562175</v>
+        <v>19.91621274540815</v>
       </c>
       <c r="Y8" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="Z8" t="n">
-        <v>2.73775942291862</v>
+        <v>2.737759423429122</v>
       </c>
       <c r="AA8" t="n">
-        <v>12.75430806918788</v>
+        <v>12.77986683288798</v>
       </c>
     </row>
     <row r="9" spans="1:27">
@@ -8604,28 +8625,28 @@
         <v>32</v>
       </c>
       <c r="C9" t="n">
-        <v>3.098781806768344</v>
+        <v>3.091953233214828</v>
       </c>
       <c r="D9" t="n">
-        <v>15.56905217381975</v>
+        <v>15.53474371825335</v>
       </c>
       <c r="E9" t="n">
-        <v>4.391145491801997</v>
+        <v>4.381469027154793</v>
       </c>
       <c r="F9" t="n">
-        <v>12.30371519696158</v>
+        <v>12.46926825473622</v>
       </c>
       <c r="G9" t="n">
-        <v>32.26391286258333</v>
+        <v>32.38548100014435</v>
       </c>
       <c r="H9" t="n">
-        <v>26.6699201341758</v>
+        <v>26.83230490006357</v>
       </c>
       <c r="I9" t="n">
-        <v>8.785734478150854</v>
+        <v>8.604923556260086</v>
       </c>
       <c r="J9" t="n">
-        <v>0.5072449932865355</v>
+        <v>0.5118520423414292</v>
       </c>
       <c r="K9" t="n">
         <v>1.182483619818803</v>
@@ -8634,49 +8655,49 @@
         <v>1.180312308138719</v>
       </c>
       <c r="M9" t="n">
-        <v>1.557447114779901</v>
+        <v>1.557447115290403</v>
       </c>
       <c r="N9" t="n">
-        <v>0.7793008699747366</v>
+        <v>0.6279803126980887</v>
       </c>
       <c r="O9" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="P9" t="n">
-        <v>3.191741749743329</v>
+        <v>3.0517474561793</v>
       </c>
       <c r="Q9" t="n">
-        <v>3.098781806768344</v>
+        <v>3.091953233214828</v>
       </c>
       <c r="R9" t="n">
-        <v>63.52890051600951</v>
+        <v>63.38890622244548</v>
       </c>
       <c r="S9" t="n">
-        <v>0.5624853349808941</v>
+        <v>0.4532648815865458</v>
       </c>
       <c r="T9" t="n">
-        <v>0.8124853349808941</v>
+        <v>0.7032648815865458</v>
       </c>
       <c r="U9" t="n">
         <v>0.08023942777181295</v>
       </c>
       <c r="V9" t="n">
-        <v>-0.1539964378800733</v>
+        <v>-0.1911040132728621</v>
       </c>
       <c r="W9" t="n">
-        <v>33.04660318715646</v>
+        <v>33.01685076744086</v>
       </c>
       <c r="X9" t="n">
-        <v>19.96019766562175</v>
+        <v>19.91621274540815</v>
       </c>
       <c r="Y9" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="Z9" t="n">
-        <v>2.73775942291862</v>
+        <v>2.737759423429122</v>
       </c>
       <c r="AA9" t="n">
-        <v>12.75430806918788</v>
+        <v>12.77986683288798</v>
       </c>
     </row>
     <row r="10" spans="1:27">
@@ -8687,28 +8708,28 @@
         <v>33</v>
       </c>
       <c r="C10" t="n">
-        <v>3.098781806768344</v>
+        <v>3.091953233214828</v>
       </c>
       <c r="D10" t="n">
-        <v>15.56905217381975</v>
+        <v>15.53474371825335</v>
       </c>
       <c r="E10" t="n">
-        <v>4.391145491801997</v>
+        <v>4.381469027154793</v>
       </c>
       <c r="F10" t="n">
-        <v>12.30371519696158</v>
+        <v>12.46926825473622</v>
       </c>
       <c r="G10" t="n">
-        <v>32.26391286258333</v>
+        <v>32.38548100014435</v>
       </c>
       <c r="H10" t="n">
-        <v>26.6699201341758</v>
+        <v>26.83230490006357</v>
       </c>
       <c r="I10" t="n">
-        <v>8.785734478150854</v>
+        <v>8.604923556260086</v>
       </c>
       <c r="J10" t="n">
-        <v>0.5072449932865355</v>
+        <v>0.5118520423414292</v>
       </c>
       <c r="K10" t="n">
         <v>1.182483619818803</v>
@@ -8717,49 +8738,49 @@
         <v>1.180312308138719</v>
       </c>
       <c r="M10" t="n">
-        <v>1.557447114779901</v>
+        <v>1.557447115290403</v>
       </c>
       <c r="N10" t="n">
-        <v>0.7793008699747366</v>
+        <v>0.6279803126980887</v>
       </c>
       <c r="O10" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="P10" t="n">
-        <v>3.191741749743329</v>
+        <v>3.0517474561793</v>
       </c>
       <c r="Q10" t="n">
-        <v>3.098781806768344</v>
+        <v>3.091953233214828</v>
       </c>
       <c r="R10" t="n">
-        <v>63.52890051600951</v>
+        <v>63.38890622244548</v>
       </c>
       <c r="S10" t="n">
-        <v>0.5624853349808941</v>
+        <v>0.4532648815865458</v>
       </c>
       <c r="T10" t="n">
-        <v>0.8124853349808941</v>
+        <v>0.7032648815865458</v>
       </c>
       <c r="U10" t="n">
         <v>0.08023942777181295</v>
       </c>
       <c r="V10" t="n">
-        <v>-0.1539964378800733</v>
+        <v>-0.1911040132728621</v>
       </c>
       <c r="W10" t="n">
-        <v>33.04660318715646</v>
+        <v>33.01685076744086</v>
       </c>
       <c r="X10" t="n">
-        <v>19.96019766562175</v>
+        <v>19.91621274540815</v>
       </c>
       <c r="Y10" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="Z10" t="n">
-        <v>2.73775942291862</v>
+        <v>2.737759423429122</v>
       </c>
       <c r="AA10" t="n">
-        <v>12.75430806918788</v>
+        <v>12.77986683288798</v>
       </c>
     </row>
     <row r="11" spans="1:27">
@@ -8770,28 +8791,28 @@
         <v>34</v>
       </c>
       <c r="C11" t="n">
-        <v>3.098781806768344</v>
+        <v>3.091953233214828</v>
       </c>
       <c r="D11" t="n">
-        <v>15.56905217381975</v>
+        <v>15.53474371825335</v>
       </c>
       <c r="E11" t="n">
-        <v>4.391145491801997</v>
+        <v>4.381469027154793</v>
       </c>
       <c r="F11" t="n">
-        <v>12.30371519696158</v>
+        <v>12.46926825473622</v>
       </c>
       <c r="G11" t="n">
-        <v>32.26391286258333</v>
+        <v>32.38548100014435</v>
       </c>
       <c r="H11" t="n">
-        <v>26.6699201341758</v>
+        <v>26.83230490006357</v>
       </c>
       <c r="I11" t="n">
-        <v>8.785734478150854</v>
+        <v>8.604923556260086</v>
       </c>
       <c r="J11" t="n">
-        <v>0.5072449932865355</v>
+        <v>0.5118520423414292</v>
       </c>
       <c r="K11" t="n">
         <v>1.182483619818803</v>
@@ -8800,49 +8821,49 @@
         <v>1.180312308138719</v>
       </c>
       <c r="M11" t="n">
-        <v>1.557447114779901</v>
+        <v>1.557447115290403</v>
       </c>
       <c r="N11" t="n">
-        <v>0.7793008699747366</v>
+        <v>0.6279803126980887</v>
       </c>
       <c r="O11" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="P11" t="n">
-        <v>3.191741749743329</v>
+        <v>3.0517474561793</v>
       </c>
       <c r="Q11" t="n">
-        <v>3.098781806768344</v>
+        <v>3.091953233214828</v>
       </c>
       <c r="R11" t="n">
-        <v>63.52890051600951</v>
+        <v>63.38890622244548</v>
       </c>
       <c r="S11" t="n">
-        <v>0.5624853349808941</v>
+        <v>0.4532648815865458</v>
       </c>
       <c r="T11" t="n">
-        <v>0.8124853349808941</v>
+        <v>0.7032648815865458</v>
       </c>
       <c r="U11" t="n">
         <v>0.08023942777181295</v>
       </c>
       <c r="V11" t="n">
-        <v>-0.1539964378800733</v>
+        <v>-0.1911040132728621</v>
       </c>
       <c r="W11" t="n">
-        <v>33.04660318715646</v>
+        <v>33.01685076744086</v>
       </c>
       <c r="X11" t="n">
-        <v>19.96019766562175</v>
+        <v>19.91621274540815</v>
       </c>
       <c r="Y11" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="Z11" t="n">
-        <v>2.73775942291862</v>
+        <v>2.737759423429122</v>
       </c>
       <c r="AA11" t="n">
-        <v>12.75430806918788</v>
+        <v>12.77986683288798</v>
       </c>
     </row>
     <row r="12" spans="1:27">
@@ -8853,28 +8874,28 @@
         <v>35</v>
       </c>
       <c r="C12" t="n">
-        <v>3.098781806768344</v>
+        <v>3.091953233214828</v>
       </c>
       <c r="D12" t="n">
-        <v>15.56905217381975</v>
+        <v>15.53474371825335</v>
       </c>
       <c r="E12" t="n">
-        <v>4.391145491801997</v>
+        <v>4.381469027154793</v>
       </c>
       <c r="F12" t="n">
-        <v>12.30371519696158</v>
+        <v>12.46926825473622</v>
       </c>
       <c r="G12" t="n">
-        <v>32.26391286258333</v>
+        <v>32.38548100014435</v>
       </c>
       <c r="H12" t="n">
-        <v>26.6699201341758</v>
+        <v>26.83230490006357</v>
       </c>
       <c r="I12" t="n">
-        <v>8.785734478150854</v>
+        <v>8.604923556260086</v>
       </c>
       <c r="J12" t="n">
-        <v>0.5072449932865355</v>
+        <v>0.5118520423414292</v>
       </c>
       <c r="K12" t="n">
         <v>1.182483619818803</v>
@@ -8883,49 +8904,49 @@
         <v>1.180312308138719</v>
       </c>
       <c r="M12" t="n">
-        <v>1.557447114779901</v>
+        <v>1.557447115290403</v>
       </c>
       <c r="N12" t="n">
-        <v>0.7793008699747366</v>
+        <v>0.6279803126980887</v>
       </c>
       <c r="O12" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="P12" t="n">
-        <v>3.191741749743329</v>
+        <v>3.0517474561793</v>
       </c>
       <c r="Q12" t="n">
-        <v>3.098781806768344</v>
+        <v>3.091953233214828</v>
       </c>
       <c r="R12" t="n">
-        <v>63.52890051600951</v>
+        <v>63.38890622244548</v>
       </c>
       <c r="S12" t="n">
-        <v>0.5624853349808941</v>
+        <v>0.4532648815865458</v>
       </c>
       <c r="T12" t="n">
-        <v>0.8124853349808941</v>
+        <v>0.7032648815865458</v>
       </c>
       <c r="U12" t="n">
         <v>0.08023942777181295</v>
       </c>
       <c r="V12" t="n">
-        <v>-0.1539964378800733</v>
+        <v>-0.1911040132728621</v>
       </c>
       <c r="W12" t="n">
-        <v>33.04660318715646</v>
+        <v>33.01685076744086</v>
       </c>
       <c r="X12" t="n">
-        <v>19.96019766562175</v>
+        <v>19.91621274540815</v>
       </c>
       <c r="Y12" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="Z12" t="n">
-        <v>2.73775942291862</v>
+        <v>2.737759423429122</v>
       </c>
       <c r="AA12" t="n">
-        <v>12.75430806918788</v>
+        <v>12.77986683288798</v>
       </c>
     </row>
     <row r="13" spans="1:27">
@@ -8936,28 +8957,28 @@
         <v>36</v>
       </c>
       <c r="C13" t="n">
-        <v>3.098781806768344</v>
+        <v>3.091953233214828</v>
       </c>
       <c r="D13" t="n">
-        <v>15.56905217381975</v>
+        <v>15.53474371825335</v>
       </c>
       <c r="E13" t="n">
-        <v>4.391145491801997</v>
+        <v>4.381469027154793</v>
       </c>
       <c r="F13" t="n">
-        <v>12.30371519696158</v>
+        <v>12.46926825473622</v>
       </c>
       <c r="G13" t="n">
-        <v>32.26391286258333</v>
+        <v>32.38548100014435</v>
       </c>
       <c r="H13" t="n">
-        <v>26.6699201341758</v>
+        <v>26.83230490006357</v>
       </c>
       <c r="I13" t="n">
-        <v>8.785734478150854</v>
+        <v>8.604923556260086</v>
       </c>
       <c r="J13" t="n">
-        <v>0.5072449932865355</v>
+        <v>0.5118520423414292</v>
       </c>
       <c r="K13" t="n">
         <v>1.182483619818803</v>
@@ -8966,49 +8987,49 @@
         <v>1.180312308138719</v>
       </c>
       <c r="M13" t="n">
-        <v>1.557447114779901</v>
+        <v>1.557447115290403</v>
       </c>
       <c r="N13" t="n">
-        <v>0.7793008699747366</v>
+        <v>0.6279803126980887</v>
       </c>
       <c r="O13" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="P13" t="n">
-        <v>3.191741749743329</v>
+        <v>3.0517474561793</v>
       </c>
       <c r="Q13" t="n">
-        <v>3.098781806768344</v>
+        <v>3.091953233214828</v>
       </c>
       <c r="R13" t="n">
-        <v>63.52890051600951</v>
+        <v>63.38890622244548</v>
       </c>
       <c r="S13" t="n">
-        <v>0.5624853349808941</v>
+        <v>0.4532648815865458</v>
       </c>
       <c r="T13" t="n">
-        <v>0.8124853349808941</v>
+        <v>0.7032648815865458</v>
       </c>
       <c r="U13" t="n">
         <v>0.08023942777181295</v>
       </c>
       <c r="V13" t="n">
-        <v>-0.1539964378800733</v>
+        <v>-0.1911040132728621</v>
       </c>
       <c r="W13" t="n">
-        <v>33.04660318715646</v>
+        <v>33.01685076744086</v>
       </c>
       <c r="X13" t="n">
-        <v>19.96019766562175</v>
+        <v>19.91621274540815</v>
       </c>
       <c r="Y13" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="Z13" t="n">
-        <v>2.73775942291862</v>
+        <v>2.737759423429122</v>
       </c>
       <c r="AA13" t="n">
-        <v>12.75430806918788</v>
+        <v>12.77986683288798</v>
       </c>
     </row>
     <row r="14" spans="1:27">
@@ -9019,79 +9040,79 @@
         <v>37</v>
       </c>
       <c r="C14" t="n">
-        <v>3.19134098912875</v>
+        <v>3.091953233214828</v>
       </c>
       <c r="D14" t="n">
-        <v>16.03409257653146</v>
+        <v>15.53474371825335</v>
       </c>
       <c r="E14" t="n">
-        <v>4.522306980958487</v>
+        <v>4.381469027154793</v>
       </c>
       <c r="F14" t="n">
-        <v>12.333181640394</v>
+        <v>12.46926825473622</v>
       </c>
       <c r="G14" t="n">
-        <v>32.88958119788393</v>
+        <v>32.38548100014435</v>
       </c>
       <c r="H14" t="n">
-        <v>25.69600771344708</v>
+        <v>26.83230490006357</v>
       </c>
       <c r="I14" t="n">
-        <v>12.28289417154646</v>
+        <v>8.604923556260086</v>
       </c>
       <c r="J14" t="n">
-        <v>0.5318428804597801</v>
+        <v>0.5118520423414292</v>
       </c>
       <c r="K14" t="n">
         <v>1.182483619818803</v>
       </c>
       <c r="L14" t="n">
-        <v>3.147499488369918</v>
+        <v>1.180312308138719</v>
       </c>
       <c r="M14" t="n">
-        <v>1.557447114779901</v>
+        <v>1.557447115290403</v>
       </c>
       <c r="N14" t="n">
-        <v>0.7793008699747366</v>
+        <v>0.6279803126980887</v>
       </c>
       <c r="O14" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="P14" t="n">
-        <v>5.089320687109604</v>
+        <v>3.0517474561793</v>
       </c>
       <c r="Q14" t="n">
-        <v>3.19134098912875</v>
+        <v>3.091953233214828</v>
       </c>
       <c r="R14" t="n">
-        <v>65.42647945337579</v>
+        <v>63.38890622244548</v>
       </c>
       <c r="S14" t="n">
-        <v>0.5624853349808941</v>
+        <v>0.4532648815865458</v>
       </c>
       <c r="T14" t="n">
-        <v>1.229152001647561</v>
+        <v>0.7032648815865458</v>
       </c>
       <c r="U14" t="n">
         <v>0.08023942777181295</v>
       </c>
       <c r="V14" t="n">
-        <v>-0.1539964378800733</v>
+        <v>-0.1911040132728621</v>
       </c>
       <c r="W14" t="n">
-        <v>33.67227152245708</v>
+        <v>33.01685076744086</v>
       </c>
       <c r="X14" t="n">
-        <v>20.55639955748994</v>
+        <v>19.91621274540815</v>
       </c>
       <c r="Y14" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="Z14" t="n">
-        <v>4.704946603149819</v>
+        <v>2.737759423429122</v>
       </c>
       <c r="AA14" t="n">
-        <v>12.71416626975537</v>
+        <v>12.77986683288798</v>
       </c>
     </row>
     <row r="15" spans="1:27">
@@ -9102,79 +9123,79 @@
         <v>38</v>
       </c>
       <c r="C15" t="n">
-        <v>3.19134098912875</v>
+        <v>3.091953233214828</v>
       </c>
       <c r="D15" t="n">
-        <v>16.03409257653146</v>
+        <v>15.53474371825335</v>
       </c>
       <c r="E15" t="n">
-        <v>4.522306980958487</v>
+        <v>4.381469027154793</v>
       </c>
       <c r="F15" t="n">
-        <v>12.333181640394</v>
+        <v>12.46926825473622</v>
       </c>
       <c r="G15" t="n">
-        <v>32.88958119788393</v>
+        <v>32.38548100014435</v>
       </c>
       <c r="H15" t="n">
-        <v>25.69600771344708</v>
+        <v>26.83230490006357</v>
       </c>
       <c r="I15" t="n">
-        <v>12.28289417154646</v>
+        <v>8.604923556260086</v>
       </c>
       <c r="J15" t="n">
-        <v>0.5318428804597801</v>
+        <v>0.5118520423414292</v>
       </c>
       <c r="K15" t="n">
         <v>1.182483619818803</v>
       </c>
       <c r="L15" t="n">
-        <v>3.147499488369918</v>
+        <v>1.180312308138719</v>
       </c>
       <c r="M15" t="n">
-        <v>1.557447114779901</v>
+        <v>1.557447115290403</v>
       </c>
       <c r="N15" t="n">
-        <v>0.7793008699747366</v>
+        <v>0.6279803126980887</v>
       </c>
       <c r="O15" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="P15" t="n">
-        <v>5.089320687109604</v>
+        <v>3.0517474561793</v>
       </c>
       <c r="Q15" t="n">
-        <v>3.19134098912875</v>
+        <v>3.091953233214828</v>
       </c>
       <c r="R15" t="n">
-        <v>65.42647945337579</v>
+        <v>63.38890622244548</v>
       </c>
       <c r="S15" t="n">
-        <v>0.5624853349808941</v>
+        <v>0.4532648815865458</v>
       </c>
       <c r="T15" t="n">
-        <v>1.229152001647561</v>
+        <v>0.7032648815865458</v>
       </c>
       <c r="U15" t="n">
         <v>0.08023942777181295</v>
       </c>
       <c r="V15" t="n">
-        <v>-0.1539964378800733</v>
+        <v>-0.1911040132728621</v>
       </c>
       <c r="W15" t="n">
-        <v>33.67227152245708</v>
+        <v>33.01685076744086</v>
       </c>
       <c r="X15" t="n">
-        <v>20.55639955748994</v>
+        <v>19.91621274540815</v>
       </c>
       <c r="Y15" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="Z15" t="n">
-        <v>4.704946603149819</v>
+        <v>2.737759423429122</v>
       </c>
       <c r="AA15" t="n">
-        <v>12.71416626975537</v>
+        <v>12.77986683288798</v>
       </c>
     </row>
     <row r="16" spans="1:27">
@@ -9185,79 +9206,79 @@
         <v>39</v>
       </c>
       <c r="C16" t="n">
-        <v>3.19134098912875</v>
+        <v>3.091953233214828</v>
       </c>
       <c r="D16" t="n">
-        <v>16.03409257653146</v>
+        <v>15.53474371825335</v>
       </c>
       <c r="E16" t="n">
-        <v>4.522306980958487</v>
+        <v>4.381469027154793</v>
       </c>
       <c r="F16" t="n">
-        <v>12.333181640394</v>
+        <v>12.46926825473622</v>
       </c>
       <c r="G16" t="n">
-        <v>32.88958119788393</v>
+        <v>32.38548100014435</v>
       </c>
       <c r="H16" t="n">
-        <v>25.69600771344708</v>
+        <v>26.83230490006357</v>
       </c>
       <c r="I16" t="n">
-        <v>12.28289417154646</v>
+        <v>8.604923556260086</v>
       </c>
       <c r="J16" t="n">
-        <v>0.5318428804597801</v>
+        <v>0.5118520423414292</v>
       </c>
       <c r="K16" t="n">
         <v>1.182483619818803</v>
       </c>
       <c r="L16" t="n">
-        <v>3.147499488369918</v>
+        <v>1.180312308138719</v>
       </c>
       <c r="M16" t="n">
-        <v>1.557447114779901</v>
+        <v>1.557447115290403</v>
       </c>
       <c r="N16" t="n">
-        <v>0.7793008699747366</v>
+        <v>0.6279803126980887</v>
       </c>
       <c r="O16" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="P16" t="n">
-        <v>5.089320687109604</v>
+        <v>3.0517474561793</v>
       </c>
       <c r="Q16" t="n">
-        <v>3.19134098912875</v>
+        <v>3.091953233214828</v>
       </c>
       <c r="R16" t="n">
-        <v>65.42647945337579</v>
+        <v>63.38890622244548</v>
       </c>
       <c r="S16" t="n">
-        <v>0.5624853349808941</v>
+        <v>0.4532648815865458</v>
       </c>
       <c r="T16" t="n">
-        <v>1.229152001647561</v>
+        <v>0.7032648815865458</v>
       </c>
       <c r="U16" t="n">
         <v>0.08023942777181295</v>
       </c>
       <c r="V16" t="n">
-        <v>-0.1539964378800733</v>
+        <v>-0.1911040132728621</v>
       </c>
       <c r="W16" t="n">
-        <v>33.67227152245708</v>
+        <v>33.01685076744086</v>
       </c>
       <c r="X16" t="n">
-        <v>20.55639955748994</v>
+        <v>19.91621274540815</v>
       </c>
       <c r="Y16" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="Z16" t="n">
-        <v>4.704946603149819</v>
+        <v>2.737759423429122</v>
       </c>
       <c r="AA16" t="n">
-        <v>12.71416626975537</v>
+        <v>12.77986683288798</v>
       </c>
     </row>
     <row r="17" spans="1:27">
@@ -9268,79 +9289,79 @@
         <v>40</v>
       </c>
       <c r="C17" t="n">
-        <v>3.19134098912875</v>
+        <v>3.091953233214828</v>
       </c>
       <c r="D17" t="n">
-        <v>16.03409257653146</v>
+        <v>15.53474371825335</v>
       </c>
       <c r="E17" t="n">
-        <v>4.522306980958487</v>
+        <v>4.381469027154793</v>
       </c>
       <c r="F17" t="n">
-        <v>12.333181640394</v>
+        <v>12.46926825473622</v>
       </c>
       <c r="G17" t="n">
-        <v>32.88958119788393</v>
+        <v>32.38548100014435</v>
       </c>
       <c r="H17" t="n">
-        <v>25.69600771344708</v>
+        <v>26.83230490006357</v>
       </c>
       <c r="I17" t="n">
-        <v>12.28289417154646</v>
+        <v>8.604923556260086</v>
       </c>
       <c r="J17" t="n">
-        <v>0.5318428804597801</v>
+        <v>0.5118520423414292</v>
       </c>
       <c r="K17" t="n">
         <v>1.182483619818803</v>
       </c>
       <c r="L17" t="n">
-        <v>3.147499488369918</v>
+        <v>1.180312308138719</v>
       </c>
       <c r="M17" t="n">
-        <v>1.557447114779901</v>
+        <v>1.557447115290403</v>
       </c>
       <c r="N17" t="n">
-        <v>0.7793008699747366</v>
+        <v>0.6279803126980887</v>
       </c>
       <c r="O17" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="P17" t="n">
-        <v>5.089320687109604</v>
+        <v>3.0517474561793</v>
       </c>
       <c r="Q17" t="n">
-        <v>3.19134098912875</v>
+        <v>3.091953233214828</v>
       </c>
       <c r="R17" t="n">
-        <v>65.42647945337579</v>
+        <v>63.38890622244548</v>
       </c>
       <c r="S17" t="n">
-        <v>0.5624853349808941</v>
+        <v>0.4532648815865458</v>
       </c>
       <c r="T17" t="n">
-        <v>1.229152001647561</v>
+        <v>0.7032648815865458</v>
       </c>
       <c r="U17" t="n">
         <v>0.08023942777181295</v>
       </c>
       <c r="V17" t="n">
-        <v>-0.1539964378800733</v>
+        <v>-0.1911040132728621</v>
       </c>
       <c r="W17" t="n">
-        <v>33.67227152245708</v>
+        <v>33.01685076744086</v>
       </c>
       <c r="X17" t="n">
-        <v>20.55639955748994</v>
+        <v>19.91621274540815</v>
       </c>
       <c r="Y17" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="Z17" t="n">
-        <v>4.704946603149819</v>
+        <v>2.737759423429122</v>
       </c>
       <c r="AA17" t="n">
-        <v>12.71416626975537</v>
+        <v>12.77986683288798</v>
       </c>
     </row>
     <row r="18" spans="1:27">
@@ -9351,79 +9372,79 @@
         <v>41</v>
       </c>
       <c r="C18" t="n">
-        <v>3.19134098912875</v>
+        <v>3.091953233214828</v>
       </c>
       <c r="D18" t="n">
-        <v>16.03409257653146</v>
+        <v>15.53474371825335</v>
       </c>
       <c r="E18" t="n">
-        <v>4.522306980958487</v>
+        <v>4.381469027154793</v>
       </c>
       <c r="F18" t="n">
-        <v>12.333181640394</v>
+        <v>12.46926825473622</v>
       </c>
       <c r="G18" t="n">
-        <v>32.88958119788393</v>
+        <v>32.38548100014435</v>
       </c>
       <c r="H18" t="n">
-        <v>25.69600771344708</v>
+        <v>26.83230490006357</v>
       </c>
       <c r="I18" t="n">
-        <v>12.28289417154646</v>
+        <v>8.604923556260086</v>
       </c>
       <c r="J18" t="n">
-        <v>0.5318428804597801</v>
+        <v>0.5118520423414292</v>
       </c>
       <c r="K18" t="n">
         <v>1.182483619818803</v>
       </c>
       <c r="L18" t="n">
-        <v>3.147499488369918</v>
+        <v>1.180312308138719</v>
       </c>
       <c r="M18" t="n">
-        <v>1.557447114779901</v>
+        <v>1.557447115290403</v>
       </c>
       <c r="N18" t="n">
-        <v>0.7793008699747366</v>
+        <v>0.6279803126980887</v>
       </c>
       <c r="O18" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="P18" t="n">
-        <v>5.089320687109604</v>
+        <v>3.0517474561793</v>
       </c>
       <c r="Q18" t="n">
-        <v>3.19134098912875</v>
+        <v>3.091953233214828</v>
       </c>
       <c r="R18" t="n">
-        <v>65.42647945337579</v>
+        <v>63.38890622244548</v>
       </c>
       <c r="S18" t="n">
-        <v>0.5624853349808941</v>
+        <v>0.4532648815865458</v>
       </c>
       <c r="T18" t="n">
-        <v>1.229152001647561</v>
+        <v>0.7032648815865458</v>
       </c>
       <c r="U18" t="n">
         <v>0.08023942777181295</v>
       </c>
       <c r="V18" t="n">
-        <v>-0.1539964378800733</v>
+        <v>-0.1911040132728621</v>
       </c>
       <c r="W18" t="n">
-        <v>33.67227152245708</v>
+        <v>33.01685076744086</v>
       </c>
       <c r="X18" t="n">
-        <v>20.55639955748994</v>
+        <v>19.91621274540815</v>
       </c>
       <c r="Y18" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="Z18" t="n">
-        <v>4.704946603149819</v>
+        <v>2.737759423429122</v>
       </c>
       <c r="AA18" t="n">
-        <v>12.71416626975537</v>
+        <v>12.77986683288798</v>
       </c>
     </row>
     <row r="19" spans="1:27">
@@ -9434,79 +9455,79 @@
         <v>42</v>
       </c>
       <c r="C19" t="n">
-        <v>3.19134098912875</v>
+        <v>3.091953233214828</v>
       </c>
       <c r="D19" t="n">
-        <v>16.03409257653146</v>
+        <v>15.53474371825335</v>
       </c>
       <c r="E19" t="n">
-        <v>4.522306980958487</v>
+        <v>4.381469027154793</v>
       </c>
       <c r="F19" t="n">
-        <v>12.333181640394</v>
+        <v>12.46926825473622</v>
       </c>
       <c r="G19" t="n">
-        <v>32.88958119788393</v>
+        <v>32.38548100014435</v>
       </c>
       <c r="H19" t="n">
-        <v>25.69600771344708</v>
+        <v>26.83230490006357</v>
       </c>
       <c r="I19" t="n">
-        <v>12.28289417154646</v>
+        <v>8.604923556260086</v>
       </c>
       <c r="J19" t="n">
-        <v>0.5318428804597801</v>
+        <v>0.5118520423414292</v>
       </c>
       <c r="K19" t="n">
         <v>1.182483619818803</v>
       </c>
       <c r="L19" t="n">
-        <v>3.147499488369918</v>
+        <v>1.180312308138719</v>
       </c>
       <c r="M19" t="n">
-        <v>1.557447114779901</v>
+        <v>1.557447115290403</v>
       </c>
       <c r="N19" t="n">
-        <v>0.7793008699747366</v>
+        <v>0.6279803126980887</v>
       </c>
       <c r="O19" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="P19" t="n">
-        <v>5.089320687109604</v>
+        <v>3.0517474561793</v>
       </c>
       <c r="Q19" t="n">
-        <v>3.19134098912875</v>
+        <v>3.091953233214828</v>
       </c>
       <c r="R19" t="n">
-        <v>65.42647945337579</v>
+        <v>63.38890622244548</v>
       </c>
       <c r="S19" t="n">
-        <v>0.5624853349808941</v>
+        <v>0.4532648815865458</v>
       </c>
       <c r="T19" t="n">
-        <v>1.229152001647561</v>
+        <v>0.7032648815865458</v>
       </c>
       <c r="U19" t="n">
         <v>0.08023942777181295</v>
       </c>
       <c r="V19" t="n">
-        <v>-0.1539964378800733</v>
+        <v>-0.1911040132728621</v>
       </c>
       <c r="W19" t="n">
-        <v>33.67227152245708</v>
+        <v>33.01685076744086</v>
       </c>
       <c r="X19" t="n">
-        <v>20.55639955748994</v>
+        <v>19.91621274540815</v>
       </c>
       <c r="Y19" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="Z19" t="n">
-        <v>4.704946603149819</v>
+        <v>2.737759423429122</v>
       </c>
       <c r="AA19" t="n">
-        <v>12.71416626975537</v>
+        <v>12.77986683288798</v>
       </c>
     </row>
     <row r="20" spans="1:27">
@@ -9517,79 +9538,79 @@
         <v>43</v>
       </c>
       <c r="C20" t="n">
-        <v>3.19134098912875</v>
+        <v>3.091953233214828</v>
       </c>
       <c r="D20" t="n">
-        <v>16.03409257653146</v>
+        <v>15.53474371825335</v>
       </c>
       <c r="E20" t="n">
-        <v>4.522306980958487</v>
+        <v>4.381469027154793</v>
       </c>
       <c r="F20" t="n">
-        <v>12.333181640394</v>
+        <v>12.46926825473622</v>
       </c>
       <c r="G20" t="n">
-        <v>32.88958119788393</v>
+        <v>32.38548100014435</v>
       </c>
       <c r="H20" t="n">
-        <v>25.69600771344708</v>
+        <v>26.83230490006357</v>
       </c>
       <c r="I20" t="n">
-        <v>12.28289417154646</v>
+        <v>8.604923556260086</v>
       </c>
       <c r="J20" t="n">
-        <v>0.5318428804597801</v>
+        <v>0.5118520423414292</v>
       </c>
       <c r="K20" t="n">
         <v>1.182483619818803</v>
       </c>
       <c r="L20" t="n">
-        <v>3.147499488369918</v>
+        <v>1.180312308138719</v>
       </c>
       <c r="M20" t="n">
-        <v>1.557447114779901</v>
+        <v>1.557447115290403</v>
       </c>
       <c r="N20" t="n">
-        <v>0.7793008699747366</v>
+        <v>0.6279803126980887</v>
       </c>
       <c r="O20" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="P20" t="n">
-        <v>5.089320687109604</v>
+        <v>3.0517474561793</v>
       </c>
       <c r="Q20" t="n">
-        <v>3.19134098912875</v>
+        <v>3.091953233214828</v>
       </c>
       <c r="R20" t="n">
-        <v>65.42647945337579</v>
+        <v>63.38890622244548</v>
       </c>
       <c r="S20" t="n">
-        <v>0.5624853349808941</v>
+        <v>0.4532648815865458</v>
       </c>
       <c r="T20" t="n">
-        <v>1.229152001647561</v>
+        <v>0.7032648815865458</v>
       </c>
       <c r="U20" t="n">
         <v>0.08023942777181295</v>
       </c>
       <c r="V20" t="n">
-        <v>-0.1539964378800733</v>
+        <v>-0.1911040132728621</v>
       </c>
       <c r="W20" t="n">
-        <v>33.67227152245708</v>
+        <v>33.01685076744086</v>
       </c>
       <c r="X20" t="n">
-        <v>20.55639955748994</v>
+        <v>19.91621274540815</v>
       </c>
       <c r="Y20" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="Z20" t="n">
-        <v>4.704946603149819</v>
+        <v>2.737759423429122</v>
       </c>
       <c r="AA20" t="n">
-        <v>12.71416626975537</v>
+        <v>12.77986683288798</v>
       </c>
     </row>
     <row r="21" spans="1:27">
@@ -9600,79 +9621,79 @@
         <v>44</v>
       </c>
       <c r="C21" t="n">
-        <v>3.19134098912875</v>
+        <v>3.061100172428026</v>
       </c>
       <c r="D21" t="n">
-        <v>16.03409257653146</v>
+        <v>15.37973025068279</v>
       </c>
       <c r="E21" t="n">
-        <v>4.522306980958487</v>
+        <v>4.337748530745557</v>
       </c>
       <c r="F21" t="n">
-        <v>12.333181640394</v>
+        <v>12.45999248566049</v>
       </c>
       <c r="G21" t="n">
-        <v>32.88958119788393</v>
+        <v>32.17747126708883</v>
       </c>
       <c r="H21" t="n">
-        <v>25.69600771344708</v>
+        <v>27.13881411214454</v>
       </c>
       <c r="I21" t="n">
-        <v>12.28289417154646</v>
+        <v>7.457878298668167</v>
       </c>
       <c r="J21" t="n">
-        <v>0.5318428804597801</v>
+        <v>0.5042105153070779</v>
       </c>
       <c r="K21" t="n">
         <v>1.182483619818803</v>
       </c>
       <c r="L21" t="n">
-        <v>3.147499488369918</v>
+        <v>0.5245832480616529</v>
       </c>
       <c r="M21" t="n">
-        <v>1.557447114779901</v>
+        <v>1.557447115290403</v>
       </c>
       <c r="N21" t="n">
-        <v>0.7793008699747366</v>
+        <v>0.6279803126980887</v>
       </c>
       <c r="O21" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="P21" t="n">
-        <v>5.089320687109604</v>
+        <v>2.419221143723876</v>
       </c>
       <c r="Q21" t="n">
-        <v>3.19134098912875</v>
+        <v>3.061100172428026</v>
       </c>
       <c r="R21" t="n">
-        <v>65.42647945337579</v>
+        <v>62.75637990999006</v>
       </c>
       <c r="S21" t="n">
-        <v>0.5624853349808941</v>
+        <v>0.4532648815865458</v>
       </c>
       <c r="T21" t="n">
-        <v>1.229152001647561</v>
+        <v>0.5643759926976569</v>
       </c>
       <c r="U21" t="n">
         <v>0.08023942777181295</v>
       </c>
       <c r="V21" t="n">
-        <v>-0.1539964378800733</v>
+        <v>-0.1911040132728621</v>
       </c>
       <c r="W21" t="n">
-        <v>33.67227152245708</v>
+        <v>32.80884103438532</v>
       </c>
       <c r="X21" t="n">
-        <v>20.55639955748994</v>
+        <v>19.71747878142834</v>
       </c>
       <c r="Y21" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="Z21" t="n">
-        <v>4.704946603149819</v>
+        <v>2.082030363352056</v>
       </c>
       <c r="AA21" t="n">
-        <v>12.71416626975537</v>
+        <v>12.79379381143391</v>
       </c>
     </row>
     <row r="22" spans="1:27">
@@ -9683,79 +9704,79 @@
         <v>45</v>
       </c>
       <c r="C22" t="n">
-        <v>3.19134098912875</v>
+        <v>3.061100172428026</v>
       </c>
       <c r="D22" t="n">
-        <v>16.03409257653146</v>
+        <v>15.37973025068279</v>
       </c>
       <c r="E22" t="n">
-        <v>4.522306980958487</v>
+        <v>4.337748530745557</v>
       </c>
       <c r="F22" t="n">
-        <v>12.333181640394</v>
+        <v>12.45999248566049</v>
       </c>
       <c r="G22" t="n">
-        <v>32.88958119788393</v>
+        <v>32.17747126708883</v>
       </c>
       <c r="H22" t="n">
-        <v>25.69600771344708</v>
+        <v>27.13881411214454</v>
       </c>
       <c r="I22" t="n">
-        <v>12.28289417154646</v>
+        <v>7.457878298668167</v>
       </c>
       <c r="J22" t="n">
-        <v>0.5318428804597801</v>
+        <v>0.5042105153070779</v>
       </c>
       <c r="K22" t="n">
         <v>1.182483619818803</v>
       </c>
       <c r="L22" t="n">
-        <v>3.147499488369918</v>
+        <v>0.5245832480616529</v>
       </c>
       <c r="M22" t="n">
-        <v>1.557447114779901</v>
+        <v>1.557447115290403</v>
       </c>
       <c r="N22" t="n">
-        <v>0.7793008699747366</v>
+        <v>0.6279803126980887</v>
       </c>
       <c r="O22" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="P22" t="n">
-        <v>5.089320687109604</v>
+        <v>2.419221143723876</v>
       </c>
       <c r="Q22" t="n">
-        <v>3.19134098912875</v>
+        <v>3.061100172428026</v>
       </c>
       <c r="R22" t="n">
-        <v>65.42647945337579</v>
+        <v>62.75637990999006</v>
       </c>
       <c r="S22" t="n">
-        <v>0.5624853349808941</v>
+        <v>0.4532648815865458</v>
       </c>
       <c r="T22" t="n">
-        <v>1.229152001647561</v>
+        <v>0.5643759926976569</v>
       </c>
       <c r="U22" t="n">
         <v>0.08023942777181295</v>
       </c>
       <c r="V22" t="n">
-        <v>-0.1539964378800733</v>
+        <v>-0.1911040132728621</v>
       </c>
       <c r="W22" t="n">
-        <v>33.67227152245708</v>
+        <v>32.80884103438532</v>
       </c>
       <c r="X22" t="n">
-        <v>20.55639955748994</v>
+        <v>19.71747878142834</v>
       </c>
       <c r="Y22" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="Z22" t="n">
-        <v>4.704946603149819</v>
+        <v>2.082030363352056</v>
       </c>
       <c r="AA22" t="n">
-        <v>12.71416626975537</v>
+        <v>12.79379381143391</v>
       </c>
     </row>
     <row r="23" spans="1:27">
@@ -9766,79 +9787,79 @@
         <v>46</v>
       </c>
       <c r="C23" t="n">
-        <v>3.19134098912875</v>
+        <v>3.061100172428026</v>
       </c>
       <c r="D23" t="n">
-        <v>16.03409257653146</v>
+        <v>15.37973025068279</v>
       </c>
       <c r="E23" t="n">
-        <v>4.522306980958487</v>
+        <v>4.337748530745557</v>
       </c>
       <c r="F23" t="n">
-        <v>12.333181640394</v>
+        <v>12.45999248566049</v>
       </c>
       <c r="G23" t="n">
-        <v>32.88958119788393</v>
+        <v>32.17747126708883</v>
       </c>
       <c r="H23" t="n">
-        <v>25.69600771344708</v>
+        <v>27.13881411214454</v>
       </c>
       <c r="I23" t="n">
-        <v>12.28289417154646</v>
+        <v>7.457878298668167</v>
       </c>
       <c r="J23" t="n">
-        <v>0.5318428804597801</v>
+        <v>0.5042105153070779</v>
       </c>
       <c r="K23" t="n">
         <v>1.182483619818803</v>
       </c>
       <c r="L23" t="n">
-        <v>3.147499488369918</v>
+        <v>0.5245832480616529</v>
       </c>
       <c r="M23" t="n">
-        <v>1.557447114779901</v>
+        <v>1.557447115290403</v>
       </c>
       <c r="N23" t="n">
-        <v>0.7793008699747366</v>
+        <v>0.6279803126980887</v>
       </c>
       <c r="O23" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="P23" t="n">
-        <v>5.089320687109604</v>
+        <v>2.419221143723876</v>
       </c>
       <c r="Q23" t="n">
-        <v>3.19134098912875</v>
+        <v>3.061100172428026</v>
       </c>
       <c r="R23" t="n">
-        <v>65.42647945337579</v>
+        <v>62.75637990999006</v>
       </c>
       <c r="S23" t="n">
-        <v>0.5624853349808941</v>
+        <v>0.4532648815865458</v>
       </c>
       <c r="T23" t="n">
-        <v>1.229152001647561</v>
+        <v>0.5643759926976569</v>
       </c>
       <c r="U23" t="n">
         <v>0.08023942777181295</v>
       </c>
       <c r="V23" t="n">
-        <v>-0.1539964378800733</v>
+        <v>-0.1911040132728621</v>
       </c>
       <c r="W23" t="n">
-        <v>33.67227152245708</v>
+        <v>32.80884103438532</v>
       </c>
       <c r="X23" t="n">
-        <v>20.55639955748994</v>
+        <v>19.71747878142834</v>
       </c>
       <c r="Y23" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="Z23" t="n">
-        <v>4.704946603149819</v>
+        <v>2.082030363352056</v>
       </c>
       <c r="AA23" t="n">
-        <v>12.71416626975537</v>
+        <v>12.79379381143391</v>
       </c>
     </row>
     <row r="24" spans="1:27">
@@ -9849,79 +9870,79 @@
         <v>47</v>
       </c>
       <c r="C24" t="n">
-        <v>3.19134098912875</v>
+        <v>3.061100172428026</v>
       </c>
       <c r="D24" t="n">
-        <v>16.03409257653146</v>
+        <v>15.37973025068279</v>
       </c>
       <c r="E24" t="n">
-        <v>4.522306980958487</v>
+        <v>4.337748530745557</v>
       </c>
       <c r="F24" t="n">
-        <v>12.333181640394</v>
+        <v>12.45999248566049</v>
       </c>
       <c r="G24" t="n">
-        <v>32.88958119788393</v>
+        <v>32.17747126708883</v>
       </c>
       <c r="H24" t="n">
-        <v>25.69600771344708</v>
+        <v>27.13881411214454</v>
       </c>
       <c r="I24" t="n">
-        <v>12.28289417154646</v>
+        <v>7.457878298668167</v>
       </c>
       <c r="J24" t="n">
-        <v>0.5318428804597801</v>
+        <v>0.5042105153070779</v>
       </c>
       <c r="K24" t="n">
         <v>1.182483619818803</v>
       </c>
       <c r="L24" t="n">
-        <v>3.147499488369918</v>
+        <v>0.5245832480616529</v>
       </c>
       <c r="M24" t="n">
-        <v>1.557447114779901</v>
+        <v>1.557447115290403</v>
       </c>
       <c r="N24" t="n">
-        <v>0.7793008699747366</v>
+        <v>0.6279803126980887</v>
       </c>
       <c r="O24" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="P24" t="n">
-        <v>5.089320687109604</v>
+        <v>2.419221143723876</v>
       </c>
       <c r="Q24" t="n">
-        <v>3.19134098912875</v>
+        <v>3.061100172428026</v>
       </c>
       <c r="R24" t="n">
-        <v>65.42647945337579</v>
+        <v>62.75637990999006</v>
       </c>
       <c r="S24" t="n">
-        <v>0.5624853349808941</v>
+        <v>0.4532648815865458</v>
       </c>
       <c r="T24" t="n">
-        <v>1.229152001647561</v>
+        <v>0.5643759926976569</v>
       </c>
       <c r="U24" t="n">
         <v>0.08023942777181295</v>
       </c>
       <c r="V24" t="n">
-        <v>-0.1539964378800733</v>
+        <v>-0.1911040132728621</v>
       </c>
       <c r="W24" t="n">
-        <v>33.67227152245708</v>
+        <v>32.80884103438532</v>
       </c>
       <c r="X24" t="n">
-        <v>20.55639955748994</v>
+        <v>19.71747878142834</v>
       </c>
       <c r="Y24" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="Z24" t="n">
-        <v>4.704946603149819</v>
+        <v>2.082030363352056</v>
       </c>
       <c r="AA24" t="n">
-        <v>12.71416626975537</v>
+        <v>12.79379381143391</v>
       </c>
     </row>
     <row r="25" spans="1:27">
@@ -9932,79 +9953,79 @@
         <v>48</v>
       </c>
       <c r="C25" t="n">
-        <v>3.376459353849562</v>
+        <v>3.061100172428026</v>
       </c>
       <c r="D25" t="n">
-        <v>16.96417338195486</v>
+        <v>15.37973025068279</v>
       </c>
       <c r="E25" t="n">
-        <v>4.784629959271467</v>
+        <v>4.337748530745557</v>
       </c>
       <c r="F25" t="n">
-        <v>12.39877635554874</v>
+        <v>12.45999248566049</v>
       </c>
       <c r="G25" t="n">
-        <v>34.14757969677508</v>
+        <v>32.17747126708883</v>
       </c>
       <c r="H25" t="n">
-        <v>23.5276815220614</v>
+        <v>27.13881411214454</v>
       </c>
       <c r="I25" t="n">
-        <v>19.50437673655584</v>
+        <v>7.457878298668167</v>
       </c>
       <c r="J25" t="n">
-        <v>0.586610233711133</v>
+        <v>0.5042105153070779</v>
       </c>
       <c r="K25" t="n">
         <v>1.182483619818803</v>
       </c>
       <c r="L25" t="n">
-        <v>7.081873848832313</v>
+        <v>0.5245832480616529</v>
       </c>
       <c r="M25" t="n">
-        <v>1.557447114779901</v>
+        <v>1.557447115290403</v>
       </c>
       <c r="N25" t="n">
-        <v>0.7793008699747366</v>
+        <v>0.6279803126980887</v>
       </c>
       <c r="O25" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="P25" t="n">
-        <v>8.884478561842151</v>
+        <v>2.419221143723876</v>
       </c>
       <c r="Q25" t="n">
-        <v>3.376459353849562</v>
+        <v>3.061100172428026</v>
       </c>
       <c r="R25" t="n">
-        <v>69.22163732810833</v>
+        <v>62.75637990999006</v>
       </c>
       <c r="S25" t="n">
-        <v>0.5624853349808941</v>
+        <v>0.4532648815865458</v>
       </c>
       <c r="T25" t="n">
-        <v>2.062485334980894</v>
+        <v>0.5643759926976569</v>
       </c>
       <c r="U25" t="n">
         <v>0.08023942777181295</v>
       </c>
       <c r="V25" t="n">
-        <v>-0.1539964378800733</v>
+        <v>-0.1911040132728621</v>
       </c>
       <c r="W25" t="n">
-        <v>34.93027002134821</v>
+        <v>32.80884103438532</v>
       </c>
       <c r="X25" t="n">
-        <v>21.74880334122633</v>
+        <v>19.71747878142834</v>
       </c>
       <c r="Y25" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="Z25" t="n">
-        <v>8.639320963612214</v>
+        <v>2.082030363352056</v>
       </c>
       <c r="AA25" t="n">
-        <v>12.64054449918028</v>
+        <v>12.79379381143391</v>
       </c>
     </row>
     <row r="26" spans="1:27">
@@ -10015,79 +10036,79 @@
         <v>49</v>
       </c>
       <c r="C26" t="n">
-        <v>3.376459353849562</v>
+        <v>3.061100172428026</v>
       </c>
       <c r="D26" t="n">
-        <v>16.96417338195486</v>
+        <v>15.37973025068279</v>
       </c>
       <c r="E26" t="n">
-        <v>4.784629959271467</v>
+        <v>4.337748530745557</v>
       </c>
       <c r="F26" t="n">
-        <v>12.39877635554874</v>
+        <v>12.45999248566049</v>
       </c>
       <c r="G26" t="n">
-        <v>34.14757969677508</v>
+        <v>32.17747126708883</v>
       </c>
       <c r="H26" t="n">
-        <v>23.5276815220614</v>
+        <v>27.13881411214454</v>
       </c>
       <c r="I26" t="n">
-        <v>19.50437673655584</v>
+        <v>7.457878298668167</v>
       </c>
       <c r="J26" t="n">
-        <v>0.586610233711133</v>
+        <v>0.5042105153070779</v>
       </c>
       <c r="K26" t="n">
         <v>1.182483619818803</v>
       </c>
       <c r="L26" t="n">
-        <v>7.081873848832313</v>
+        <v>0.5245832480616529</v>
       </c>
       <c r="M26" t="n">
-        <v>1.557447114779901</v>
+        <v>1.557447115290403</v>
       </c>
       <c r="N26" t="n">
-        <v>0.7793008699747366</v>
+        <v>0.6279803126980887</v>
       </c>
       <c r="O26" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="P26" t="n">
-        <v>8.884478561842151</v>
+        <v>2.419221143723876</v>
       </c>
       <c r="Q26" t="n">
-        <v>3.376459353849562</v>
+        <v>3.061100172428026</v>
       </c>
       <c r="R26" t="n">
-        <v>69.22163732810833</v>
+        <v>62.75637990999006</v>
       </c>
       <c r="S26" t="n">
-        <v>0.5624853349808941</v>
+        <v>0.4532648815865458</v>
       </c>
       <c r="T26" t="n">
-        <v>2.062485334980894</v>
+        <v>0.5643759926976569</v>
       </c>
       <c r="U26" t="n">
         <v>0.08023942777181295</v>
       </c>
       <c r="V26" t="n">
-        <v>-0.1539964378800733</v>
+        <v>-0.1911040132728621</v>
       </c>
       <c r="W26" t="n">
-        <v>34.93027002134821</v>
+        <v>32.80884103438532</v>
       </c>
       <c r="X26" t="n">
-        <v>21.74880334122633</v>
+        <v>19.71747878142834</v>
       </c>
       <c r="Y26" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="Z26" t="n">
-        <v>8.639320963612214</v>
+        <v>2.082030363352056</v>
       </c>
       <c r="AA26" t="n">
-        <v>12.64054449918028</v>
+        <v>12.79379381143391</v>
       </c>
     </row>
     <row r="27" spans="1:27">
@@ -10098,79 +10119,79 @@
         <v>50</v>
       </c>
       <c r="C27" t="n">
-        <v>3.376459353849562</v>
+        <v>3.061100172428026</v>
       </c>
       <c r="D27" t="n">
-        <v>16.96417338195486</v>
+        <v>15.37973025068279</v>
       </c>
       <c r="E27" t="n">
-        <v>4.784629959271467</v>
+        <v>4.337748530745557</v>
       </c>
       <c r="F27" t="n">
-        <v>12.39877635554874</v>
+        <v>12.45999248566049</v>
       </c>
       <c r="G27" t="n">
-        <v>34.14757969677508</v>
+        <v>32.17747126708883</v>
       </c>
       <c r="H27" t="n">
-        <v>23.5276815220614</v>
+        <v>27.13881411214454</v>
       </c>
       <c r="I27" t="n">
-        <v>19.50437673655584</v>
+        <v>7.457878298668167</v>
       </c>
       <c r="J27" t="n">
-        <v>0.586610233711133</v>
+        <v>0.5042105153070779</v>
       </c>
       <c r="K27" t="n">
         <v>1.182483619818803</v>
       </c>
       <c r="L27" t="n">
-        <v>7.081873848832313</v>
+        <v>0.5245832480616529</v>
       </c>
       <c r="M27" t="n">
-        <v>1.557447114779901</v>
+        <v>1.557447115290403</v>
       </c>
       <c r="N27" t="n">
-        <v>0.7793008699747366</v>
+        <v>0.6279803126980887</v>
       </c>
       <c r="O27" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="P27" t="n">
-        <v>8.884478561842151</v>
+        <v>2.419221143723876</v>
       </c>
       <c r="Q27" t="n">
-        <v>3.376459353849562</v>
+        <v>3.061100172428026</v>
       </c>
       <c r="R27" t="n">
-        <v>69.22163732810833</v>
+        <v>62.75637990999006</v>
       </c>
       <c r="S27" t="n">
-        <v>0.5624853349808941</v>
+        <v>0.4532648815865458</v>
       </c>
       <c r="T27" t="n">
-        <v>2.062485334980894</v>
+        <v>0.5643759926976569</v>
       </c>
       <c r="U27" t="n">
         <v>0.08023942777181295</v>
       </c>
       <c r="V27" t="n">
-        <v>-0.1539964378800733</v>
+        <v>-0.1911040132728621</v>
       </c>
       <c r="W27" t="n">
-        <v>34.93027002134821</v>
+        <v>32.80884103438532</v>
       </c>
       <c r="X27" t="n">
-        <v>21.74880334122633</v>
+        <v>19.71747878142834</v>
       </c>
       <c r="Y27" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="Z27" t="n">
-        <v>8.639320963612214</v>
+        <v>2.082030363352056</v>
       </c>
       <c r="AA27" t="n">
-        <v>12.64054449918028</v>
+        <v>12.79379381143391</v>
       </c>
     </row>
     <row r="28" spans="1:27">
@@ -10181,79 +10202,79 @@
         <v>51</v>
       </c>
       <c r="C28" t="n">
-        <v>3.376459353849562</v>
+        <v>3.061100172428026</v>
       </c>
       <c r="D28" t="n">
-        <v>16.96417338195486</v>
+        <v>15.37973025068279</v>
       </c>
       <c r="E28" t="n">
-        <v>4.784629959271467</v>
+        <v>4.337748530745557</v>
       </c>
       <c r="F28" t="n">
-        <v>12.39877635554874</v>
+        <v>12.45999248566049</v>
       </c>
       <c r="G28" t="n">
-        <v>34.14757969677508</v>
+        <v>32.17747126708883</v>
       </c>
       <c r="H28" t="n">
-        <v>23.5276815220614</v>
+        <v>27.13881411214454</v>
       </c>
       <c r="I28" t="n">
-        <v>19.50437673655584</v>
+        <v>7.457878298668167</v>
       </c>
       <c r="J28" t="n">
-        <v>0.586610233711133</v>
+        <v>0.5042105153070779</v>
       </c>
       <c r="K28" t="n">
         <v>1.182483619818803</v>
       </c>
       <c r="L28" t="n">
-        <v>7.081873848832313</v>
+        <v>0.5245832480616529</v>
       </c>
       <c r="M28" t="n">
-        <v>1.557447114779901</v>
+        <v>1.557447115290403</v>
       </c>
       <c r="N28" t="n">
-        <v>0.7793008699747366</v>
+        <v>0.6279803126980887</v>
       </c>
       <c r="O28" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="P28" t="n">
-        <v>8.884478561842151</v>
+        <v>2.419221143723876</v>
       </c>
       <c r="Q28" t="n">
-        <v>3.376459353849562</v>
+        <v>3.061100172428026</v>
       </c>
       <c r="R28" t="n">
-        <v>69.22163732810833</v>
+        <v>62.75637990999006</v>
       </c>
       <c r="S28" t="n">
-        <v>0.5624853349808941</v>
+        <v>0.4532648815865458</v>
       </c>
       <c r="T28" t="n">
-        <v>2.062485334980894</v>
+        <v>0.5643759926976569</v>
       </c>
       <c r="U28" t="n">
         <v>0.08023942777181295</v>
       </c>
       <c r="V28" t="n">
-        <v>-0.1539964378800733</v>
+        <v>-0.1911040132728621</v>
       </c>
       <c r="W28" t="n">
-        <v>34.93027002134821</v>
+        <v>32.80884103438532</v>
       </c>
       <c r="X28" t="n">
-        <v>21.74880334122633</v>
+        <v>19.71747878142834</v>
       </c>
       <c r="Y28" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="Z28" t="n">
-        <v>8.639320963612214</v>
+        <v>2.082030363352056</v>
       </c>
       <c r="AA28" t="n">
-        <v>12.64054449918028</v>
+        <v>12.79379381143391</v>
       </c>
     </row>
     <row r="29" spans="1:27">
@@ -10264,79 +10285,79 @@
         <v>52</v>
       </c>
       <c r="C29" t="n">
-        <v>3.376459353849562</v>
+        <v>3.061100172428026</v>
       </c>
       <c r="D29" t="n">
-        <v>16.96417338195486</v>
+        <v>15.37973025068279</v>
       </c>
       <c r="E29" t="n">
-        <v>4.784629959271467</v>
+        <v>4.337748530745557</v>
       </c>
       <c r="F29" t="n">
-        <v>12.39877635554874</v>
+        <v>12.45999248566049</v>
       </c>
       <c r="G29" t="n">
-        <v>34.14757969677508</v>
+        <v>32.17747126708883</v>
       </c>
       <c r="H29" t="n">
-        <v>23.5276815220614</v>
+        <v>27.13881411214454</v>
       </c>
       <c r="I29" t="n">
-        <v>19.50437673655584</v>
+        <v>7.457878298668167</v>
       </c>
       <c r="J29" t="n">
-        <v>0.586610233711133</v>
+        <v>0.5042105153070779</v>
       </c>
       <c r="K29" t="n">
         <v>1.182483619818803</v>
       </c>
       <c r="L29" t="n">
-        <v>7.081873848832313</v>
+        <v>0.5245832480616529</v>
       </c>
       <c r="M29" t="n">
-        <v>1.557447114779901</v>
+        <v>1.557447115290403</v>
       </c>
       <c r="N29" t="n">
-        <v>0.7793008699747366</v>
+        <v>0.6279803126980887</v>
       </c>
       <c r="O29" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="P29" t="n">
-        <v>8.884478561842151</v>
+        <v>2.419221143723876</v>
       </c>
       <c r="Q29" t="n">
-        <v>3.376459353849562</v>
+        <v>3.061100172428026</v>
       </c>
       <c r="R29" t="n">
-        <v>69.22163732810833</v>
+        <v>62.75637990999006</v>
       </c>
       <c r="S29" t="n">
-        <v>0.5624853349808941</v>
+        <v>0.4532648815865458</v>
       </c>
       <c r="T29" t="n">
-        <v>2.062485334980894</v>
+        <v>0.5643759926976569</v>
       </c>
       <c r="U29" t="n">
         <v>0.08023942777181295</v>
       </c>
       <c r="V29" t="n">
-        <v>-0.1539964378800733</v>
+        <v>-0.1911040132728621</v>
       </c>
       <c r="W29" t="n">
-        <v>34.93027002134821</v>
+        <v>32.80884103438532</v>
       </c>
       <c r="X29" t="n">
-        <v>21.74880334122633</v>
+        <v>19.71747878142834</v>
       </c>
       <c r="Y29" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="Z29" t="n">
-        <v>8.639320963612214</v>
+        <v>2.082030363352056</v>
       </c>
       <c r="AA29" t="n">
-        <v>12.64054449918028</v>
+        <v>12.79379381143391</v>
       </c>
     </row>
     <row r="30" spans="1:27">
@@ -10347,79 +10368,79 @@
         <v>53</v>
       </c>
       <c r="C30" t="n">
-        <v>3.376459353849562</v>
+        <v>3.061100172428026</v>
       </c>
       <c r="D30" t="n">
-        <v>16.96417338195486</v>
+        <v>15.37973025068279</v>
       </c>
       <c r="E30" t="n">
-        <v>4.784629959271467</v>
+        <v>4.337748530745557</v>
       </c>
       <c r="F30" t="n">
-        <v>12.39877635554874</v>
+        <v>12.45999248566049</v>
       </c>
       <c r="G30" t="n">
-        <v>34.14757969677508</v>
+        <v>32.17747126708883</v>
       </c>
       <c r="H30" t="n">
-        <v>23.5276815220614</v>
+        <v>27.13881411214454</v>
       </c>
       <c r="I30" t="n">
-        <v>19.50437673655584</v>
+        <v>7.457878298668167</v>
       </c>
       <c r="J30" t="n">
-        <v>0.586610233711133</v>
+        <v>0.5042105153070779</v>
       </c>
       <c r="K30" t="n">
         <v>1.182483619818803</v>
       </c>
       <c r="L30" t="n">
-        <v>7.081873848832313</v>
+        <v>0.5245832480616529</v>
       </c>
       <c r="M30" t="n">
-        <v>1.557447114779901</v>
+        <v>1.557447115290403</v>
       </c>
       <c r="N30" t="n">
-        <v>0.7793008699747366</v>
+        <v>0.6279803126980887</v>
       </c>
       <c r="O30" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="P30" t="n">
-        <v>8.884478561842151</v>
+        <v>2.419221143723876</v>
       </c>
       <c r="Q30" t="n">
-        <v>3.376459353849562</v>
+        <v>3.061100172428026</v>
       </c>
       <c r="R30" t="n">
-        <v>69.22163732810833</v>
+        <v>62.75637990999006</v>
       </c>
       <c r="S30" t="n">
-        <v>0.5624853349808941</v>
+        <v>0.4532648815865458</v>
       </c>
       <c r="T30" t="n">
-        <v>2.062485334980894</v>
+        <v>0.5643759926976569</v>
       </c>
       <c r="U30" t="n">
         <v>0.08023942777181295</v>
       </c>
       <c r="V30" t="n">
-        <v>-0.1539964378800733</v>
+        <v>-0.1911040132728621</v>
       </c>
       <c r="W30" t="n">
-        <v>34.93027002134821</v>
+        <v>32.80884103438532</v>
       </c>
       <c r="X30" t="n">
-        <v>21.74880334122633</v>
+        <v>19.71747878142834</v>
       </c>
       <c r="Y30" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="Z30" t="n">
-        <v>8.639320963612214</v>
+        <v>2.082030363352056</v>
       </c>
       <c r="AA30" t="n">
-        <v>12.64054449918028</v>
+        <v>12.79379381143391</v>
       </c>
     </row>
     <row r="31" spans="1:27">
@@ -10430,79 +10451,79 @@
         <v>54</v>
       </c>
       <c r="C31" t="n">
-        <v>3.376459353849562</v>
+        <v>3.061100172428026</v>
       </c>
       <c r="D31" t="n">
-        <v>16.96417338195486</v>
+        <v>15.37973025068279</v>
       </c>
       <c r="E31" t="n">
-        <v>4.784629959271467</v>
+        <v>4.337748530745557</v>
       </c>
       <c r="F31" t="n">
-        <v>12.39877635554874</v>
+        <v>12.45999248566049</v>
       </c>
       <c r="G31" t="n">
-        <v>34.14757969677508</v>
+        <v>32.17747126708883</v>
       </c>
       <c r="H31" t="n">
-        <v>23.5276815220614</v>
+        <v>27.13881411214454</v>
       </c>
       <c r="I31" t="n">
-        <v>19.50437673655584</v>
+        <v>7.457878298668167</v>
       </c>
       <c r="J31" t="n">
-        <v>0.586610233711133</v>
+        <v>0.5042105153070779</v>
       </c>
       <c r="K31" t="n">
         <v>1.182483619818803</v>
       </c>
       <c r="L31" t="n">
-        <v>7.081873848832313</v>
+        <v>0.5245832480616529</v>
       </c>
       <c r="M31" t="n">
-        <v>1.557447114779901</v>
+        <v>1.557447115290403</v>
       </c>
       <c r="N31" t="n">
-        <v>0.7793008699747366</v>
+        <v>0.6279803126980887</v>
       </c>
       <c r="O31" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="P31" t="n">
-        <v>8.884478561842151</v>
+        <v>2.419221143723876</v>
       </c>
       <c r="Q31" t="n">
-        <v>3.376459353849562</v>
+        <v>3.061100172428026</v>
       </c>
       <c r="R31" t="n">
-        <v>69.22163732810833</v>
+        <v>62.75637990999006</v>
       </c>
       <c r="S31" t="n">
-        <v>0.5624853349808941</v>
+        <v>0.4532648815865458</v>
       </c>
       <c r="T31" t="n">
-        <v>2.062485334980894</v>
+        <v>0.5643759926976569</v>
       </c>
       <c r="U31" t="n">
         <v>0.08023942777181295</v>
       </c>
       <c r="V31" t="n">
-        <v>-0.1539964378800733</v>
+        <v>-0.1911040132728621</v>
       </c>
       <c r="W31" t="n">
-        <v>34.93027002134821</v>
+        <v>32.80884103438532</v>
       </c>
       <c r="X31" t="n">
-        <v>21.74880334122633</v>
+        <v>19.71747878142834</v>
       </c>
       <c r="Y31" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="Z31" t="n">
-        <v>8.639320963612214</v>
+        <v>2.082030363352056</v>
       </c>
       <c r="AA31" t="n">
-        <v>12.64054449918028</v>
+        <v>12.79379381143391</v>
       </c>
     </row>
     <row r="32" spans="1:27">
@@ -10513,79 +10534,79 @@
         <v>55</v>
       </c>
       <c r="C32" t="n">
-        <v>3.376459353849562</v>
+        <v>3.061100172428026</v>
       </c>
       <c r="D32" t="n">
-        <v>16.96417338195486</v>
+        <v>15.37973025068279</v>
       </c>
       <c r="E32" t="n">
-        <v>4.784629959271467</v>
+        <v>4.337748530745557</v>
       </c>
       <c r="F32" t="n">
-        <v>12.39877635554874</v>
+        <v>12.45999248566049</v>
       </c>
       <c r="G32" t="n">
-        <v>34.14757969677508</v>
+        <v>32.17747126708883</v>
       </c>
       <c r="H32" t="n">
-        <v>23.5276815220614</v>
+        <v>27.13881411214454</v>
       </c>
       <c r="I32" t="n">
-        <v>19.50437673655584</v>
+        <v>7.457878298668167</v>
       </c>
       <c r="J32" t="n">
-        <v>0.586610233711133</v>
+        <v>0.5042105153070779</v>
       </c>
       <c r="K32" t="n">
         <v>1.182483619818803</v>
       </c>
       <c r="L32" t="n">
-        <v>7.081873848832313</v>
+        <v>0.5245832480616529</v>
       </c>
       <c r="M32" t="n">
-        <v>1.557447114779901</v>
+        <v>1.557447115290403</v>
       </c>
       <c r="N32" t="n">
-        <v>0.7793008699747366</v>
+        <v>0.6279803126980887</v>
       </c>
       <c r="O32" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="P32" t="n">
-        <v>8.884478561842151</v>
+        <v>2.419221143723876</v>
       </c>
       <c r="Q32" t="n">
-        <v>3.376459353849562</v>
+        <v>3.061100172428026</v>
       </c>
       <c r="R32" t="n">
-        <v>69.22163732810833</v>
+        <v>62.75637990999006</v>
       </c>
       <c r="S32" t="n">
-        <v>0.5624853349808941</v>
+        <v>0.4532648815865458</v>
       </c>
       <c r="T32" t="n">
-        <v>2.062485334980894</v>
+        <v>0.5643759926976569</v>
       </c>
       <c r="U32" t="n">
         <v>0.08023942777181295</v>
       </c>
       <c r="V32" t="n">
-        <v>-0.1539964378800733</v>
+        <v>-0.1911040132728621</v>
       </c>
       <c r="W32" t="n">
-        <v>34.93027002134821</v>
+        <v>32.80884103438532</v>
       </c>
       <c r="X32" t="n">
-        <v>21.74880334122633</v>
+        <v>19.71747878142834</v>
       </c>
       <c r="Y32" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="Z32" t="n">
-        <v>8.639320963612214</v>
+        <v>2.082030363352056</v>
       </c>
       <c r="AA32" t="n">
-        <v>12.64054449918028</v>
+        <v>12.79379381143391</v>
       </c>
     </row>
     <row r="33" spans="1:27">
@@ -10596,79 +10617,79 @@
         <v>56</v>
       </c>
       <c r="C33" t="n">
-        <v>3.376459353849562</v>
+        <v>3.061100172428026</v>
       </c>
       <c r="D33" t="n">
-        <v>16.96417338195486</v>
+        <v>15.37973025068279</v>
       </c>
       <c r="E33" t="n">
-        <v>4.784629959271467</v>
+        <v>4.337748530745557</v>
       </c>
       <c r="F33" t="n">
-        <v>12.39877635554874</v>
+        <v>12.45999248566049</v>
       </c>
       <c r="G33" t="n">
-        <v>34.14757969677508</v>
+        <v>32.17747126708883</v>
       </c>
       <c r="H33" t="n">
-        <v>23.5276815220614</v>
+        <v>27.13881411214454</v>
       </c>
       <c r="I33" t="n">
-        <v>19.50437673655584</v>
+        <v>7.457878298668167</v>
       </c>
       <c r="J33" t="n">
-        <v>0.586610233711133</v>
+        <v>0.5042105153070779</v>
       </c>
       <c r="K33" t="n">
         <v>1.182483619818803</v>
       </c>
       <c r="L33" t="n">
-        <v>7.081873848832313</v>
+        <v>0.5245832480616529</v>
       </c>
       <c r="M33" t="n">
-        <v>1.557447114779901</v>
+        <v>1.557447115290403</v>
       </c>
       <c r="N33" t="n">
-        <v>0.7793008699747366</v>
+        <v>0.6279803126980887</v>
       </c>
       <c r="O33" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="P33" t="n">
-        <v>8.884478561842151</v>
+        <v>2.419221143723876</v>
       </c>
       <c r="Q33" t="n">
-        <v>3.376459353849562</v>
+        <v>3.061100172428026</v>
       </c>
       <c r="R33" t="n">
-        <v>69.22163732810833</v>
+        <v>62.75637990999006</v>
       </c>
       <c r="S33" t="n">
-        <v>0.5624853349808941</v>
+        <v>0.4532648815865458</v>
       </c>
       <c r="T33" t="n">
-        <v>2.062485334980894</v>
+        <v>0.5643759926976569</v>
       </c>
       <c r="U33" t="n">
         <v>0.08023942777181295</v>
       </c>
       <c r="V33" t="n">
-        <v>-0.1539964378800733</v>
+        <v>-0.1911040132728621</v>
       </c>
       <c r="W33" t="n">
-        <v>34.93027002134821</v>
+        <v>32.80884103438532</v>
       </c>
       <c r="X33" t="n">
-        <v>21.74880334122633</v>
+        <v>19.71747878142834</v>
       </c>
       <c r="Y33" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="Z33" t="n">
-        <v>8.639320963612214</v>
+        <v>2.082030363352056</v>
       </c>
       <c r="AA33" t="n">
-        <v>12.64054449918028</v>
+        <v>12.79379381143391</v>
       </c>
     </row>
     <row r="34" spans="1:27">
@@ -10679,79 +10700,79 @@
         <v>57</v>
       </c>
       <c r="C34" t="n">
-        <v>3.376459353849562</v>
+        <v>3.061100172428026</v>
       </c>
       <c r="D34" t="n">
-        <v>16.96417338195486</v>
+        <v>15.37973025068279</v>
       </c>
       <c r="E34" t="n">
-        <v>4.784629959271467</v>
+        <v>4.337748530745557</v>
       </c>
       <c r="F34" t="n">
-        <v>12.39877635554874</v>
+        <v>12.45999248566049</v>
       </c>
       <c r="G34" t="n">
-        <v>34.14757969677508</v>
+        <v>32.17747126708883</v>
       </c>
       <c r="H34" t="n">
-        <v>23.5276815220614</v>
+        <v>27.13881411214454</v>
       </c>
       <c r="I34" t="n">
-        <v>19.50437673655584</v>
+        <v>7.457878298668167</v>
       </c>
       <c r="J34" t="n">
-        <v>0.586610233711133</v>
+        <v>0.5042105153070779</v>
       </c>
       <c r="K34" t="n">
         <v>1.182483619818803</v>
       </c>
       <c r="L34" t="n">
-        <v>7.081873848832313</v>
+        <v>0.5245832480616529</v>
       </c>
       <c r="M34" t="n">
-        <v>1.557447114779901</v>
+        <v>1.557447115290403</v>
       </c>
       <c r="N34" t="n">
-        <v>0.7793008699747366</v>
+        <v>0.6279803126980887</v>
       </c>
       <c r="O34" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="P34" t="n">
-        <v>8.884478561842151</v>
+        <v>2.419221143723876</v>
       </c>
       <c r="Q34" t="n">
-        <v>3.376459353849562</v>
+        <v>3.061100172428026</v>
       </c>
       <c r="R34" t="n">
-        <v>69.22163732810833</v>
+        <v>62.75637990999006</v>
       </c>
       <c r="S34" t="n">
-        <v>0.5624853349808941</v>
+        <v>0.4532648815865458</v>
       </c>
       <c r="T34" t="n">
-        <v>2.062485334980894</v>
+        <v>0.5643759926976569</v>
       </c>
       <c r="U34" t="n">
         <v>0.08023942777181295</v>
       </c>
       <c r="V34" t="n">
-        <v>-0.1539964378800733</v>
+        <v>-0.1911040132728621</v>
       </c>
       <c r="W34" t="n">
-        <v>34.93027002134821</v>
+        <v>32.80884103438532</v>
       </c>
       <c r="X34" t="n">
-        <v>21.74880334122633</v>
+        <v>19.71747878142834</v>
       </c>
       <c r="Y34" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="Z34" t="n">
-        <v>8.639320963612214</v>
+        <v>2.082030363352056</v>
       </c>
       <c r="AA34" t="n">
-        <v>12.64054449918028</v>
+        <v>12.79379381143391</v>
       </c>
     </row>
     <row r="35" spans="1:27">
@@ -10762,79 +10783,660 @@
         <v>58</v>
       </c>
       <c r="C35" t="n">
-        <v>3.376459353849562</v>
+        <v>3.061100172428026</v>
       </c>
       <c r="D35" t="n">
-        <v>16.96417338195486</v>
+        <v>15.37973025068279</v>
       </c>
       <c r="E35" t="n">
-        <v>4.784629959271467</v>
+        <v>4.337748530745557</v>
       </c>
       <c r="F35" t="n">
-        <v>12.39877635554874</v>
+        <v>12.45999248566049</v>
       </c>
       <c r="G35" t="n">
-        <v>34.14757969677508</v>
+        <v>32.17747126708883</v>
       </c>
       <c r="H35" t="n">
-        <v>23.5276815220614</v>
+        <v>27.13881411214454</v>
       </c>
       <c r="I35" t="n">
-        <v>19.50437673655584</v>
+        <v>7.457878298668167</v>
       </c>
       <c r="J35" t="n">
-        <v>0.586610233711133</v>
+        <v>0.5042105153070779</v>
       </c>
       <c r="K35" t="n">
         <v>1.182483619818803</v>
       </c>
       <c r="L35" t="n">
-        <v>7.081873848832313</v>
+        <v>0.5245832480616529</v>
       </c>
       <c r="M35" t="n">
-        <v>1.557447114779901</v>
+        <v>1.557447115290403</v>
       </c>
       <c r="N35" t="n">
-        <v>0.7793008699747366</v>
+        <v>0.6279803126980887</v>
       </c>
       <c r="O35" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="P35" t="n">
-        <v>8.884478561842151</v>
+        <v>2.419221143723876</v>
       </c>
       <c r="Q35" t="n">
-        <v>3.376459353849562</v>
+        <v>3.061100172428026</v>
       </c>
       <c r="R35" t="n">
-        <v>69.22163732810833</v>
+        <v>62.75637990999006</v>
       </c>
       <c r="S35" t="n">
-        <v>0.5624853349808941</v>
+        <v>0.4532648815865458</v>
       </c>
       <c r="T35" t="n">
-        <v>2.062485334980894</v>
+        <v>0.5643759926976569</v>
       </c>
       <c r="U35" t="n">
         <v>0.08023942777181295</v>
       </c>
       <c r="V35" t="n">
-        <v>-0.1539964378800733</v>
+        <v>-0.1911040132728621</v>
       </c>
       <c r="W35" t="n">
-        <v>34.93027002134821</v>
+        <v>32.80884103438532</v>
       </c>
       <c r="X35" t="n">
-        <v>21.74880334122633</v>
+        <v>19.71747878142834</v>
       </c>
       <c r="Y35" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="Z35" t="n">
-        <v>8.639320963612214</v>
+        <v>2.082030363352056</v>
       </c>
       <c r="AA35" t="n">
-        <v>12.64054449918028</v>
+        <v>12.79379381143391</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27">
+      <c r="A36" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B36" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" t="n">
+        <v>3.061100172428026</v>
+      </c>
+      <c r="D36" t="n">
+        <v>15.37973025068279</v>
+      </c>
+      <c r="E36" t="n">
+        <v>4.337748530745557</v>
+      </c>
+      <c r="F36" t="n">
+        <v>12.45999248566049</v>
+      </c>
+      <c r="G36" t="n">
+        <v>32.17747126708883</v>
+      </c>
+      <c r="H36" t="n">
+        <v>27.13881411214454</v>
+      </c>
+      <c r="I36" t="n">
+        <v>7.457878298668167</v>
+      </c>
+      <c r="J36" t="n">
+        <v>0.5042105153070779</v>
+      </c>
+      <c r="K36" t="n">
+        <v>1.182483619818803</v>
+      </c>
+      <c r="L36" t="n">
+        <v>0.5245832480616529</v>
+      </c>
+      <c r="M36" t="n">
+        <v>1.557447115290403</v>
+      </c>
+      <c r="N36" t="n">
+        <v>0.6279803126980887</v>
+      </c>
+      <c r="O36" t="n">
+        <v>0.003389454598402244</v>
+      </c>
+      <c r="P36" t="n">
+        <v>2.419221143723876</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>3.061100172428026</v>
+      </c>
+      <c r="R36" t="n">
+        <v>62.75637990999006</v>
+      </c>
+      <c r="S36" t="n">
+        <v>0.4532648815865458</v>
+      </c>
+      <c r="T36" t="n">
+        <v>0.5643759926976569</v>
+      </c>
+      <c r="U36" t="n">
+        <v>0.08023942777181295</v>
+      </c>
+      <c r="V36" t="n">
+        <v>-0.1911040132728621</v>
+      </c>
+      <c r="W36" t="n">
+        <v>32.80884103438532</v>
+      </c>
+      <c r="X36" t="n">
+        <v>19.71747878142834</v>
+      </c>
+      <c r="Y36" t="n">
+        <v>0.003389454598402244</v>
+      </c>
+      <c r="Z36" t="n">
+        <v>2.082030363352056</v>
+      </c>
+      <c r="AA36" t="n">
+        <v>12.79379381143391</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27">
+      <c r="A37" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B37" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37" t="n">
+        <v>3.061100172428026</v>
+      </c>
+      <c r="D37" t="n">
+        <v>15.37973025068279</v>
+      </c>
+      <c r="E37" t="n">
+        <v>4.337748530745557</v>
+      </c>
+      <c r="F37" t="n">
+        <v>12.45999248566049</v>
+      </c>
+      <c r="G37" t="n">
+        <v>32.17747126708883</v>
+      </c>
+      <c r="H37" t="n">
+        <v>27.13881411214454</v>
+      </c>
+      <c r="I37" t="n">
+        <v>7.457878298668167</v>
+      </c>
+      <c r="J37" t="n">
+        <v>0.5042105153070779</v>
+      </c>
+      <c r="K37" t="n">
+        <v>1.182483619818803</v>
+      </c>
+      <c r="L37" t="n">
+        <v>0.5245832480616529</v>
+      </c>
+      <c r="M37" t="n">
+        <v>1.557447115290403</v>
+      </c>
+      <c r="N37" t="n">
+        <v>0.6279803126980887</v>
+      </c>
+      <c r="O37" t="n">
+        <v>0.003389454598402244</v>
+      </c>
+      <c r="P37" t="n">
+        <v>2.419221143723876</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>3.061100172428026</v>
+      </c>
+      <c r="R37" t="n">
+        <v>62.75637990999006</v>
+      </c>
+      <c r="S37" t="n">
+        <v>0.4532648815865458</v>
+      </c>
+      <c r="T37" t="n">
+        <v>0.5643759926976569</v>
+      </c>
+      <c r="U37" t="n">
+        <v>0.08023942777181295</v>
+      </c>
+      <c r="V37" t="n">
+        <v>-0.1911040132728621</v>
+      </c>
+      <c r="W37" t="n">
+        <v>32.80884103438532</v>
+      </c>
+      <c r="X37" t="n">
+        <v>19.71747878142834</v>
+      </c>
+      <c r="Y37" t="n">
+        <v>0.003389454598402244</v>
+      </c>
+      <c r="Z37" t="n">
+        <v>2.082030363352056</v>
+      </c>
+      <c r="AA37" t="n">
+        <v>12.79379381143391</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27">
+      <c r="A38" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B38" t="s">
+        <v>61</v>
+      </c>
+      <c r="C38" t="n">
+        <v>3.067928745916581</v>
+      </c>
+      <c r="D38" t="n">
+        <v>15.4140387059228</v>
+      </c>
+      <c r="E38" t="n">
+        <v>4.347424997685081</v>
+      </c>
+      <c r="F38" t="n">
+        <v>12.29438619456033</v>
+      </c>
+      <c r="G38" t="n">
+        <v>32.0558498981682</v>
+      </c>
+      <c r="H38" t="n">
+        <v>26.97822591639774</v>
+      </c>
+      <c r="I38" t="n">
+        <v>7.636839417726588</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0.4994584175068205</v>
+      </c>
+      <c r="K38" t="n">
+        <v>1.182483619818803</v>
+      </c>
+      <c r="L38" t="n">
+        <v>0.5245832480616529</v>
+      </c>
+      <c r="M38" t="n">
+        <v>1.557447115290403</v>
+      </c>
+      <c r="N38" t="n">
+        <v>0.7793008699747366</v>
+      </c>
+      <c r="O38" t="n">
+        <v>0.003389454598402244</v>
+      </c>
+      <c r="P38" t="n">
+        <v>2.559215435956125</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>3.067928745916581</v>
+      </c>
+      <c r="R38" t="n">
+        <v>62.8963742022223</v>
+      </c>
+      <c r="S38" t="n">
+        <v>0.5624853349808941</v>
+      </c>
+      <c r="T38" t="n">
+        <v>0.6735964460920053</v>
+      </c>
+      <c r="U38" t="n">
+        <v>0.08023942777181295</v>
+      </c>
+      <c r="V38" t="n">
+        <v>-0.1539964378800733</v>
+      </c>
+      <c r="W38" t="n">
+        <v>32.83854022274134</v>
+      </c>
+      <c r="X38" t="n">
+        <v>19.76146370360788</v>
+      </c>
+      <c r="Y38" t="n">
+        <v>0.003389454598402244</v>
+      </c>
+      <c r="Z38" t="n">
+        <v>2.082030363352056</v>
+      </c>
+      <c r="AA38" t="n">
+        <v>12.768181812566</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27">
+      <c r="A39" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B39" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" t="n">
+        <v>3.067928745916581</v>
+      </c>
+      <c r="D39" t="n">
+        <v>15.4140387059228</v>
+      </c>
+      <c r="E39" t="n">
+        <v>4.347424997685081</v>
+      </c>
+      <c r="F39" t="n">
+        <v>12.29438619456033</v>
+      </c>
+      <c r="G39" t="n">
+        <v>32.0558498981682</v>
+      </c>
+      <c r="H39" t="n">
+        <v>26.97822591639774</v>
+      </c>
+      <c r="I39" t="n">
+        <v>7.636839417726588</v>
+      </c>
+      <c r="J39" t="n">
+        <v>0.4994584175068205</v>
+      </c>
+      <c r="K39" t="n">
+        <v>1.182483619818803</v>
+      </c>
+      <c r="L39" t="n">
+        <v>0.5245832480616529</v>
+      </c>
+      <c r="M39" t="n">
+        <v>1.557447115290403</v>
+      </c>
+      <c r="N39" t="n">
+        <v>0.7793008699747366</v>
+      </c>
+      <c r="O39" t="n">
+        <v>0.003389454598402244</v>
+      </c>
+      <c r="P39" t="n">
+        <v>2.559215435956125</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>3.067928745916581</v>
+      </c>
+      <c r="R39" t="n">
+        <v>62.8963742022223</v>
+      </c>
+      <c r="S39" t="n">
+        <v>0.5624853349808941</v>
+      </c>
+      <c r="T39" t="n">
+        <v>0.6735964460920053</v>
+      </c>
+      <c r="U39" t="n">
+        <v>0.08023942777181295</v>
+      </c>
+      <c r="V39" t="n">
+        <v>-0.1539964378800733</v>
+      </c>
+      <c r="W39" t="n">
+        <v>32.83854022274134</v>
+      </c>
+      <c r="X39" t="n">
+        <v>19.76146370360788</v>
+      </c>
+      <c r="Y39" t="n">
+        <v>0.003389454598402244</v>
+      </c>
+      <c r="Z39" t="n">
+        <v>2.082030363352056</v>
+      </c>
+      <c r="AA39" t="n">
+        <v>12.768181812566</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27">
+      <c r="A40" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B40" t="s">
+        <v>63</v>
+      </c>
+      <c r="C40" t="n">
+        <v>3.067928745916581</v>
+      </c>
+      <c r="D40" t="n">
+        <v>15.4140387059228</v>
+      </c>
+      <c r="E40" t="n">
+        <v>4.347424997685081</v>
+      </c>
+      <c r="F40" t="n">
+        <v>12.29438619456033</v>
+      </c>
+      <c r="G40" t="n">
+        <v>32.0558498981682</v>
+      </c>
+      <c r="H40" t="n">
+        <v>26.97822591639774</v>
+      </c>
+      <c r="I40" t="n">
+        <v>7.636839417726588</v>
+      </c>
+      <c r="J40" t="n">
+        <v>0.4994584175068205</v>
+      </c>
+      <c r="K40" t="n">
+        <v>1.182483619818803</v>
+      </c>
+      <c r="L40" t="n">
+        <v>0.5245832480616529</v>
+      </c>
+      <c r="M40" t="n">
+        <v>1.557447115290403</v>
+      </c>
+      <c r="N40" t="n">
+        <v>0.7793008699747366</v>
+      </c>
+      <c r="O40" t="n">
+        <v>0.003389454598402244</v>
+      </c>
+      <c r="P40" t="n">
+        <v>2.559215435956125</v>
+      </c>
+      <c r="Q40" t="n">
+        <v>3.067928745916581</v>
+      </c>
+      <c r="R40" t="n">
+        <v>62.8963742022223</v>
+      </c>
+      <c r="S40" t="n">
+        <v>0.5624853349808941</v>
+      </c>
+      <c r="T40" t="n">
+        <v>0.6735964460920053</v>
+      </c>
+      <c r="U40" t="n">
+        <v>0.08023942777181295</v>
+      </c>
+      <c r="V40" t="n">
+        <v>-0.1539964378800733</v>
+      </c>
+      <c r="W40" t="n">
+        <v>32.83854022274134</v>
+      </c>
+      <c r="X40" t="n">
+        <v>19.76146370360788</v>
+      </c>
+      <c r="Y40" t="n">
+        <v>0.003389454598402244</v>
+      </c>
+      <c r="Z40" t="n">
+        <v>2.082030363352056</v>
+      </c>
+      <c r="AA40" t="n">
+        <v>12.768181812566</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27">
+      <c r="A41" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B41" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" t="n">
+        <v>3.067928745916581</v>
+      </c>
+      <c r="D41" t="n">
+        <v>15.4140387059228</v>
+      </c>
+      <c r="E41" t="n">
+        <v>4.347424997685081</v>
+      </c>
+      <c r="F41" t="n">
+        <v>12.29438619456033</v>
+      </c>
+      <c r="G41" t="n">
+        <v>32.0558498981682</v>
+      </c>
+      <c r="H41" t="n">
+        <v>26.97822591639774</v>
+      </c>
+      <c r="I41" t="n">
+        <v>7.636839417726588</v>
+      </c>
+      <c r="J41" t="n">
+        <v>0.4994584175068205</v>
+      </c>
+      <c r="K41" t="n">
+        <v>1.182483619818803</v>
+      </c>
+      <c r="L41" t="n">
+        <v>0.5245832480616529</v>
+      </c>
+      <c r="M41" t="n">
+        <v>1.557447115290403</v>
+      </c>
+      <c r="N41" t="n">
+        <v>0.7793008699747366</v>
+      </c>
+      <c r="O41" t="n">
+        <v>0.003389454598402244</v>
+      </c>
+      <c r="P41" t="n">
+        <v>2.559215435956125</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>3.067928745916581</v>
+      </c>
+      <c r="R41" t="n">
+        <v>62.8963742022223</v>
+      </c>
+      <c r="S41" t="n">
+        <v>0.5624853349808941</v>
+      </c>
+      <c r="T41" t="n">
+        <v>0.6735964460920053</v>
+      </c>
+      <c r="U41" t="n">
+        <v>0.08023942777181295</v>
+      </c>
+      <c r="V41" t="n">
+        <v>-0.1539964378800733</v>
+      </c>
+      <c r="W41" t="n">
+        <v>32.83854022274134</v>
+      </c>
+      <c r="X41" t="n">
+        <v>19.76146370360788</v>
+      </c>
+      <c r="Y41" t="n">
+        <v>0.003389454598402244</v>
+      </c>
+      <c r="Z41" t="n">
+        <v>2.082030363352056</v>
+      </c>
+      <c r="AA41" t="n">
+        <v>12.768181812566</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27">
+      <c r="A42" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B42" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" t="n">
+        <v>3.067928745916581</v>
+      </c>
+      <c r="D42" t="n">
+        <v>15.4140387059228</v>
+      </c>
+      <c r="E42" t="n">
+        <v>4.347424997685081</v>
+      </c>
+      <c r="F42" t="n">
+        <v>12.29438619456033</v>
+      </c>
+      <c r="G42" t="n">
+        <v>32.0558498981682</v>
+      </c>
+      <c r="H42" t="n">
+        <v>26.97822591639774</v>
+      </c>
+      <c r="I42" t="n">
+        <v>7.636839417726588</v>
+      </c>
+      <c r="J42" t="n">
+        <v>0.4994584175068205</v>
+      </c>
+      <c r="K42" t="n">
+        <v>1.182483619818803</v>
+      </c>
+      <c r="L42" t="n">
+        <v>0.5245832480616529</v>
+      </c>
+      <c r="M42" t="n">
+        <v>1.557447115290403</v>
+      </c>
+      <c r="N42" t="n">
+        <v>0.7793008699747366</v>
+      </c>
+      <c r="O42" t="n">
+        <v>0.003389454598402244</v>
+      </c>
+      <c r="P42" t="n">
+        <v>2.559215435956125</v>
+      </c>
+      <c r="Q42" t="n">
+        <v>3.067928745916581</v>
+      </c>
+      <c r="R42" t="n">
+        <v>62.8963742022223</v>
+      </c>
+      <c r="S42" t="n">
+        <v>0.5624853349808941</v>
+      </c>
+      <c r="T42" t="n">
+        <v>0.6735964460920053</v>
+      </c>
+      <c r="U42" t="n">
+        <v>0.08023942777181295</v>
+      </c>
+      <c r="V42" t="n">
+        <v>-0.1539964378800733</v>
+      </c>
+      <c r="W42" t="n">
+        <v>32.83854022274134</v>
+      </c>
+      <c r="X42" t="n">
+        <v>19.76146370360788</v>
+      </c>
+      <c r="Y42" t="n">
+        <v>0.003389454598402244</v>
+      </c>
+      <c r="Z42" t="n">
+        <v>2.082030363352056</v>
+      </c>
+      <c r="AA42" t="n">
+        <v>12.768181812566</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ny data och omstrukturering
</commit_message>
<xml_diff>
--- a/masterProject/test.xlsx
+++ b/masterProject/test.xlsx
@@ -11032,28 +11032,28 @@
         <v>61</v>
       </c>
       <c r="C38" t="n">
-        <v>3.067928745916581</v>
+        <v>3.061100172428026</v>
       </c>
       <c r="D38" t="n">
-        <v>15.4140387059228</v>
+        <v>15.37973025068279</v>
       </c>
       <c r="E38" t="n">
-        <v>4.347424997685081</v>
+        <v>4.337748530745557</v>
       </c>
       <c r="F38" t="n">
-        <v>12.29438619456033</v>
+        <v>12.45999248566049</v>
       </c>
       <c r="G38" t="n">
-        <v>32.0558498981682</v>
+        <v>32.17747126708883</v>
       </c>
       <c r="H38" t="n">
-        <v>26.97822591639774</v>
+        <v>27.13881411214454</v>
       </c>
       <c r="I38" t="n">
-        <v>7.636839417726588</v>
+        <v>7.457878298668167</v>
       </c>
       <c r="J38" t="n">
-        <v>0.4994584175068205</v>
+        <v>0.5042105153070779</v>
       </c>
       <c r="K38" t="n">
         <v>1.182483619818803</v>
@@ -11065,37 +11065,37 @@
         <v>1.557447115290403</v>
       </c>
       <c r="N38" t="n">
-        <v>0.7793008699747366</v>
+        <v>0.6279803126980887</v>
       </c>
       <c r="O38" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="P38" t="n">
-        <v>2.559215435956125</v>
+        <v>2.419221143723876</v>
       </c>
       <c r="Q38" t="n">
-        <v>3.067928745916581</v>
+        <v>3.061100172428026</v>
       </c>
       <c r="R38" t="n">
-        <v>62.8963742022223</v>
+        <v>62.75637990999006</v>
       </c>
       <c r="S38" t="n">
-        <v>0.5624853349808941</v>
+        <v>0.4532648815865458</v>
       </c>
       <c r="T38" t="n">
-        <v>0.6735964460920053</v>
+        <v>0.5643759926976569</v>
       </c>
       <c r="U38" t="n">
         <v>0.08023942777181295</v>
       </c>
       <c r="V38" t="n">
-        <v>-0.1539964378800733</v>
+        <v>-0.1911040132728621</v>
       </c>
       <c r="W38" t="n">
-        <v>32.83854022274134</v>
+        <v>32.80884103438532</v>
       </c>
       <c r="X38" t="n">
-        <v>19.76146370360788</v>
+        <v>19.71747878142834</v>
       </c>
       <c r="Y38" t="n">
         <v>0.003389454598402244</v>
@@ -11104,7 +11104,7 @@
         <v>2.082030363352056</v>
       </c>
       <c r="AA38" t="n">
-        <v>12.768181812566</v>
+        <v>12.79379381143391</v>
       </c>
     </row>
     <row r="39" spans="1:27">
@@ -11115,79 +11115,79 @@
         <v>62</v>
       </c>
       <c r="C39" t="n">
-        <v>3.067928745916581</v>
+        <v>3.098976908803056</v>
       </c>
       <c r="D39" t="n">
-        <v>15.4140387059228</v>
+        <v>15.57003241507165</v>
       </c>
       <c r="E39" t="n">
-        <v>4.347424997685081</v>
+        <v>4.391421964578305</v>
       </c>
       <c r="F39" t="n">
-        <v>12.29438619456033</v>
+        <v>12.29898522126248</v>
       </c>
       <c r="G39" t="n">
-        <v>32.0558498981682</v>
+        <v>32.26043960091244</v>
       </c>
       <c r="H39" t="n">
-        <v>26.97822591639774</v>
+        <v>26.66527476125871</v>
       </c>
       <c r="I39" t="n">
-        <v>7.636839417726588</v>
+        <v>8.790906424986197</v>
       </c>
       <c r="J39" t="n">
-        <v>0.4994584175068205</v>
+        <v>0.5071117505196556</v>
       </c>
       <c r="K39" t="n">
         <v>1.182483619818803</v>
       </c>
       <c r="L39" t="n">
-        <v>0.5245832480616529</v>
+        <v>1.180312308138719</v>
       </c>
       <c r="M39" t="n">
         <v>1.557447115290403</v>
       </c>
       <c r="N39" t="n">
-        <v>0.7793008699747366</v>
+        <v>0.783624314468355</v>
       </c>
       <c r="O39" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="P39" t="n">
-        <v>2.559215435956125</v>
+        <v>3.19574158533247</v>
       </c>
       <c r="Q39" t="n">
-        <v>3.067928745916581</v>
+        <v>3.098976908803056</v>
       </c>
       <c r="R39" t="n">
-        <v>62.8963742022223</v>
+        <v>63.53290035159866</v>
       </c>
       <c r="S39" t="n">
-        <v>0.5624853349808941</v>
+        <v>0.5656059193635897</v>
       </c>
       <c r="T39" t="n">
-        <v>0.6735964460920053</v>
+        <v>0.8156059193635897</v>
       </c>
       <c r="U39" t="n">
         <v>0.08023942777181295</v>
       </c>
       <c r="V39" t="n">
-        <v>-0.1539964378800733</v>
+        <v>-0.153146802360735</v>
       </c>
       <c r="W39" t="n">
-        <v>32.83854022274134</v>
+        <v>33.04745336997919</v>
       </c>
       <c r="X39" t="n">
-        <v>19.76146370360788</v>
+        <v>19.96145437964996</v>
       </c>
       <c r="Y39" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="Z39" t="n">
-        <v>2.082030363352056</v>
+        <v>2.737759423429122</v>
       </c>
       <c r="AA39" t="n">
-        <v>12.768181812566</v>
+        <v>12.75357792856742</v>
       </c>
     </row>
     <row r="40" spans="1:27">
@@ -11198,34 +11198,34 @@
         <v>63</v>
       </c>
       <c r="C40" t="n">
-        <v>3.067928745916581</v>
+        <v>3.098781806703383</v>
       </c>
       <c r="D40" t="n">
-        <v>15.4140387059228</v>
+        <v>15.56905217349337</v>
       </c>
       <c r="E40" t="n">
-        <v>4.347424997685081</v>
+        <v>4.391145494094316</v>
       </c>
       <c r="F40" t="n">
-        <v>12.29438619456033</v>
+        <v>12.30371514166842</v>
       </c>
       <c r="G40" t="n">
-        <v>32.0558498981682</v>
+        <v>32.2639128092561</v>
       </c>
       <c r="H40" t="n">
-        <v>26.97822591639774</v>
+        <v>26.66992013483354</v>
       </c>
       <c r="I40" t="n">
-        <v>7.636839417726588</v>
+        <v>8.785734422834107</v>
       </c>
       <c r="J40" t="n">
-        <v>0.4994584175068205</v>
+        <v>0.5072449932699233</v>
       </c>
       <c r="K40" t="n">
         <v>1.182483619818803</v>
       </c>
       <c r="L40" t="n">
-        <v>0.5245832480616529</v>
+        <v>1.180312308138719</v>
       </c>
       <c r="M40" t="n">
         <v>1.557447115290403</v>
@@ -11237,19 +11237,19 @@
         <v>0.003389454598402244</v>
       </c>
       <c r="P40" t="n">
-        <v>2.559215435956125</v>
+        <v>3.191741748411549</v>
       </c>
       <c r="Q40" t="n">
-        <v>3.067928745916581</v>
+        <v>3.098781806703383</v>
       </c>
       <c r="R40" t="n">
-        <v>62.8963742022223</v>
+        <v>63.52890051467773</v>
       </c>
       <c r="S40" t="n">
         <v>0.5624853349808941</v>
       </c>
       <c r="T40" t="n">
-        <v>0.6735964460920053</v>
+        <v>0.8124853349808941</v>
       </c>
       <c r="U40" t="n">
         <v>0.08023942777181295</v>
@@ -11258,19 +11258,19 @@
         <v>-0.1539964378800733</v>
       </c>
       <c r="W40" t="n">
-        <v>32.83854022274134</v>
+        <v>33.04660313382924</v>
       </c>
       <c r="X40" t="n">
-        <v>19.76146370360788</v>
+        <v>19.96019766758768</v>
       </c>
       <c r="Y40" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="Z40" t="n">
-        <v>2.082030363352056</v>
+        <v>2.737759423429122</v>
       </c>
       <c r="AA40" t="n">
-        <v>12.768181812566</v>
+        <v>12.75430801205244</v>
       </c>
     </row>
     <row r="41" spans="1:27">
@@ -11281,28 +11281,28 @@
         <v>64</v>
       </c>
       <c r="C41" t="n">
-        <v>3.067928745916581</v>
+        <v>3.068123848016254</v>
       </c>
       <c r="D41" t="n">
-        <v>15.4140387059228</v>
+        <v>15.41501894750109</v>
       </c>
       <c r="E41" t="n">
-        <v>4.347424997685081</v>
+        <v>4.347701468169067</v>
       </c>
       <c r="F41" t="n">
-        <v>12.29438619456033</v>
+        <v>12.28965475459361</v>
       </c>
       <c r="G41" t="n">
-        <v>32.0558498981682</v>
+        <v>32.05237517026375</v>
       </c>
       <c r="H41" t="n">
-        <v>26.97822591639774</v>
+        <v>26.97363187478792</v>
       </c>
       <c r="I41" t="n">
-        <v>7.636839417726588</v>
+        <v>7.641958568352877</v>
       </c>
       <c r="J41" t="n">
-        <v>0.4994584175068205</v>
+        <v>0.4993209750534031</v>
       </c>
       <c r="K41" t="n">
         <v>1.182483619818803</v>
@@ -11314,37 +11314,37 @@
         <v>1.557447115290403</v>
       </c>
       <c r="N41" t="n">
-        <v>0.7793008699747366</v>
+        <v>0.783624314468355</v>
       </c>
       <c r="O41" t="n">
         <v>0.003389454598402244</v>
       </c>
       <c r="P41" t="n">
-        <v>2.559215435956125</v>
+        <v>2.563215272877046</v>
       </c>
       <c r="Q41" t="n">
-        <v>3.067928745916581</v>
+        <v>3.068123848016254</v>
       </c>
       <c r="R41" t="n">
-        <v>62.8963742022223</v>
+        <v>62.90037403914323</v>
       </c>
       <c r="S41" t="n">
-        <v>0.5624853349808941</v>
+        <v>0.5656059193635897</v>
       </c>
       <c r="T41" t="n">
-        <v>0.6735964460920053</v>
+        <v>0.6767170304747009</v>
       </c>
       <c r="U41" t="n">
         <v>0.08023942777181295</v>
       </c>
       <c r="V41" t="n">
-        <v>-0.1539964378800733</v>
+        <v>-0.153146802360735</v>
       </c>
       <c r="W41" t="n">
-        <v>32.83854022274134</v>
+        <v>32.83938893933052</v>
       </c>
       <c r="X41" t="n">
-        <v>19.76146370360788</v>
+        <v>19.76272041567015</v>
       </c>
       <c r="Y41" t="n">
         <v>0.003389454598402244</v>
@@ -11353,7 +11353,7 @@
         <v>2.082030363352056</v>
       </c>
       <c r="AA41" t="n">
-        <v>12.768181812566</v>
+        <v>12.76745020952018</v>
       </c>
     </row>
     <row r="42" spans="1:27">

</xml_diff>